<commit_message>
Mejoras importantes: filtros interactivos, correcciones de citas y nuevo vendedor
 Funcionalidades agregadas:
- Filtros dinámicos en matrices (horario, compradores/vendedores, búsqueda)
- Sistema de verificación exhaustiva de citas (verificar_agenda.py)
- Corrección manual de 5 citas incorrectas (100% precisión alcanzada)
- Nuevo vendedor: FINCA LA FEDERICA con 7 citas programadas

 Mejoras técnicas:
- Interfaz de filtrado responsive e intuitiva
- Actualización automática de estadísticas
- Controles de limpiar filtros
- Documentación de errores (ERRORES_DETECTADOS.md)

 Estado actual:
- 32 vendedores, 11 compradores, 65 citas programadas
- D'CLEO COFFEE  BOX BRAND programada en primer slot
- Todas las citas validadas contra preferencias originales
</commit_message>
<xml_diff>
--- a/agenda_rueda_negocios.xlsx
+++ b/agenda_rueda_negocios.xlsx
@@ -45,7 +45,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill/>
     </fill>
@@ -100,6 +100,12 @@
         <bgColor rgb="00D5F4E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FDF2F2"/>
+        <bgColor rgb="00FDF2F2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -119,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -140,6 +146,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -541,7 +548,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
@@ -627,7 +634,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13"/>
@@ -645,7 +652,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16">
@@ -655,7 +662,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17">
@@ -666,7 +673,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>350.0%</t>
+          <t>361.1%</t>
         </is>
       </c>
     </row>
@@ -678,7 +685,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>4.7</t>
         </is>
       </c>
     </row>
@@ -690,7 +697,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.9</t>
         </is>
       </c>
     </row>
@@ -702,7 +709,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>139/138</t>
+          <t>145/145</t>
         </is>
       </c>
     </row>
@@ -714,7 +721,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>100.7%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
@@ -732,7 +739,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,7 +752,7 @@
     <col width="50" customWidth="1" min="3" max="3"/>
     <col width="47" customWidth="1" min="4" max="4"/>
     <col width="47" customWidth="1" min="5" max="5"/>
-    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="47" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -817,7 +824,7 @@
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>FLOR A FRUTO</t>
+          <t>INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="D3" s="7" t="inlineStr">
@@ -873,17 +880,17 @@
       </c>
       <c r="C5" s="6" t="inlineStr">
         <is>
-          <t>REGIONAL S.A.S</t>
+          <t>COLFRESH COFFEE</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">
         <is>
+          <t>CAFÉ ERMITAÑO</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
+        <is>
           <t>CAFÉ MATILDE 1960</t>
-        </is>
-      </c>
-      <c r="E5" s="7" t="inlineStr">
-        <is>
-          <t>DELUXE COFFEE</t>
         </is>
       </c>
       <c r="F5" s="7" t="n"/>
@@ -906,12 +913,12 @@
       </c>
       <c r="D6" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ ERMITAÑO</t>
+          <t>CAFÉ GRANADA</t>
         </is>
       </c>
       <c r="E6" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ GRANADA</t>
+          <t>CAFÉ LA AVANZANTE</t>
         </is>
       </c>
       <c r="F6" s="7" t="n"/>
@@ -929,22 +936,22 @@
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>COLFRESH COFFEE</t>
+          <t>PROCOLOMBIA</t>
         </is>
       </c>
       <c r="D7" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ MURAL</t>
+          <t>FINCA LA RIVERA</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
         <is>
-          <t>EL ORGASMO DE LOS SAINOS</t>
+          <t>CAFE ARTE</t>
         </is>
       </c>
       <c r="F7" s="7" t="inlineStr">
         <is>
-          <t>LA PATRONA</t>
+          <t>CAFE FINCA MI TERRON</t>
         </is>
       </c>
     </row>
@@ -961,22 +968,22 @@
       </c>
       <c r="C8" s="6" t="inlineStr">
         <is>
-          <t>PROCOLOMBIA</t>
+          <t>REGIONAL S.A.S</t>
         </is>
       </c>
       <c r="D8" s="7" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA</t>
+          <t>DELUXE COFFEE</t>
         </is>
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>CAFE ARTE</t>
+          <t>DON HEBER CAFÉ</t>
         </is>
       </c>
       <c r="F8" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ LA AVANZANTE</t>
+          <t>EL ORGASMO DE LOS SAINOS</t>
         </is>
       </c>
     </row>
@@ -993,22 +1000,22 @@
       </c>
       <c r="C9" s="6" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS</t>
+          <t>ARMANDO VELÁSQUEZ</t>
         </is>
       </c>
       <c r="D9" s="7" t="inlineStr">
         <is>
-          <t>CAFE FINCA MI TERRON</t>
+          <t>CINCO DAMAS</t>
         </is>
       </c>
       <c r="E9" s="7" t="inlineStr">
         <is>
-          <t>CAFE MIS TAITAS</t>
+          <t>FINCA EL CASCABEL</t>
         </is>
       </c>
       <c r="F9" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ TRADICIÓN NEIRA</t>
+          <t>LADERAS DEL TAPIAS</t>
         </is>
       </c>
     </row>
@@ -1025,22 +1032,22 @@
       </c>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>ARMANDO VELÁSQUEZ</t>
+          <t>FLOR A FRUTO</t>
         </is>
       </c>
       <c r="D10" s="7" t="inlineStr">
         <is>
-          <t>CINCO DAMAS</t>
+          <t>CAFÉ CAMPOHERMOSO</t>
         </is>
       </c>
       <c r="E10" s="7" t="inlineStr">
         <is>
-          <t>DON HEBER CAFÉ</t>
+          <t>CAFÉ OASIS DE SAMDA</t>
         </is>
       </c>
       <c r="F10" s="7" t="inlineStr">
         <is>
-          <t>FINCA EL CASCABEL</t>
+          <t>RUNA COFFEE</t>
         </is>
       </c>
     </row>
@@ -1062,12 +1069,12 @@
       </c>
       <c r="D11" s="7" t="inlineStr">
         <is>
-          <t>LADERAS DEL TAPIAS</t>
+          <t>CAFÉ MURAL</t>
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr">
         <is>
-          <t>RUNA COFFEE</t>
+          <t>CAFÉ TRADICIÓN NEIRA</t>
         </is>
       </c>
       <c r="F11" s="7" t="n"/>
@@ -1085,17 +1092,17 @@
       </c>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS</t>
+          <t>INMERSSO BOUTIQUE</t>
         </is>
       </c>
       <c r="D12" s="7" t="inlineStr">
         <is>
-          <t>FINCA EL CASCABEL</t>
+          <t>RUNA COFFEE</t>
         </is>
       </c>
       <c r="E12" s="7" t="inlineStr">
         <is>
-          <t>LA PATRONA</t>
+          <t>CINCO DAMAS</t>
         </is>
       </c>
       <c r="F12" s="7" t="n"/>
@@ -1113,17 +1120,17 @@
       </c>
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>INMERSSO BOUTIQUE</t>
+          <t>CAFÉ MOLINA</t>
         </is>
       </c>
       <c r="D13" s="7" t="inlineStr">
         <is>
-          <t>CINCO DAMAS</t>
+          <t>DELUXE COFFEE</t>
         </is>
       </c>
       <c r="E13" s="7" t="inlineStr">
         <is>
-          <t>DON HEBER CAFÉ</t>
+          <t>ROJO PASIÓN</t>
         </is>
       </c>
       <c r="F13" s="7" t="n"/>
@@ -1141,12 +1148,12 @@
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>CAFÉ MOLINA</t>
+          <t>COLFRESH COFFEE</t>
         </is>
       </c>
       <c r="D14" s="7" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA</t>
+          <t>CAFÉ VALLE DE LIRIO</t>
         </is>
       </c>
       <c r="E14" s="7" t="inlineStr">
@@ -1169,7 +1176,7 @@
       </c>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>COLFRESH COFFEE</t>
+          <t>REGIONAL S.A.S</t>
         </is>
       </c>
       <c r="D15" s="7" t="inlineStr">
@@ -1179,7 +1186,7 @@
       </c>
       <c r="E15" s="7" t="inlineStr">
         <is>
-          <t>DE SOL A SOL</t>
+          <t>FINCA LA FEDERICA</t>
         </is>
       </c>
       <c r="F15" s="7" t="n"/>
@@ -1197,17 +1204,17 @@
       </c>
       <c r="C16" s="6" t="inlineStr">
         <is>
-          <t>REGIONAL S.A.S</t>
+          <t>FLOR A FRUTO</t>
         </is>
       </c>
       <c r="D16" s="7" t="inlineStr">
         <is>
-          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS</t>
+          <t>FINCA EL CASCABEL</t>
         </is>
       </c>
       <c r="E16" s="7" t="inlineStr">
         <is>
-          <t>ROJO PASIÓN</t>
+          <t>CAFÉ ARENILLO</t>
         </is>
       </c>
       <c r="F16" s="7" t="n"/>
@@ -1230,12 +1237,12 @@
       </c>
       <c r="D17" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ VALLE DE LIRIO</t>
+          <t>DON HEBER CAFÉ</t>
         </is>
       </c>
       <c r="E17" s="7" t="inlineStr">
         <is>
-          <t>DELUXE COFFEE</t>
+          <t>CAFE FINCA MI TERRON</t>
         </is>
       </c>
       <c r="F17" s="7" t="n"/>
@@ -1253,17 +1260,17 @@
       </c>
       <c r="C18" s="6" t="inlineStr">
         <is>
-          <t>FLOR A FRUTO</t>
+          <t>INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="D18" s="7" t="inlineStr">
         <is>
-          <t>SANTA CRUZ DE LAS AGUAS</t>
+          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS</t>
         </is>
       </c>
       <c r="E18" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ ERMITAÑO</t>
+          <t>CAFÉ GRANADA</t>
         </is>
       </c>
       <c r="F18" s="7" t="n"/>
@@ -1271,27 +1278,27 @@
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>08:45 - 09:00</t>
+          <t>09:00 - 09:15</t>
         </is>
       </c>
       <c r="B19" s="5" t="inlineStr">
         <is>
-          <t>Cita 9</t>
+          <t>Cita 1</t>
         </is>
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>PROCOLOMBIA</t>
+          <t>BOX BRAND</t>
         </is>
       </c>
       <c r="D19" s="7" t="inlineStr">
         <is>
-          <t>D'CLEO COFFEE</t>
+          <t>DELUXE COFFEE</t>
         </is>
       </c>
       <c r="E19" s="7" t="inlineStr">
         <is>
-          <t>EL ORGASMO DE LOS SAINOS</t>
+          <t>LADERAS DEL TAPIAS</t>
         </is>
       </c>
       <c r="F19" s="7" t="n"/>
@@ -1304,22 +1311,22 @@
       </c>
       <c r="B20" s="5" t="inlineStr">
         <is>
-          <t>Cita 1</t>
+          <t>Cita 2</t>
         </is>
       </c>
       <c r="C20" s="6" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS</t>
+          <t>INMERSSO BOUTIQUE</t>
         </is>
       </c>
       <c r="D20" s="7" t="inlineStr">
         <is>
-          <t>D'CLEO COFFEE</t>
+          <t>FINCA LA RIVERA</t>
         </is>
       </c>
       <c r="E20" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ GRANADA</t>
+          <t>ROJO PASIÓN</t>
         </is>
       </c>
       <c r="F20" s="7" t="n"/>
@@ -1332,22 +1339,22 @@
       </c>
       <c r="B21" s="5" t="inlineStr">
         <is>
-          <t>Cita 2</t>
+          <t>Cita 3</t>
         </is>
       </c>
       <c r="C21" s="6" t="inlineStr">
         <is>
-          <t>BOX BRAND</t>
+          <t>CAFÉ MOLINA</t>
         </is>
       </c>
       <c r="D21" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ MATILDE 1960</t>
+          <t>FINCA LA FEDERICA</t>
         </is>
       </c>
       <c r="E21" s="7" t="inlineStr">
         <is>
-          <t>SANTA CRUZ DE LAS AGUAS</t>
+          <t>CAFÉ AGUA VIVA</t>
         </is>
       </c>
       <c r="F21" s="7" t="n"/>
@@ -1360,25 +1367,29 @@
       </c>
       <c r="B22" s="5" t="inlineStr">
         <is>
-          <t>Cita 3</t>
+          <t>Cita 4</t>
         </is>
       </c>
       <c r="C22" s="6" t="inlineStr">
         <is>
-          <t>INMERSSO BOUTIQUE</t>
+          <t>COLFRESH COFFEE</t>
         </is>
       </c>
       <c r="D22" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ LA AVANZANTE</t>
+          <t>CAFÉ ARENILLO</t>
         </is>
       </c>
       <c r="E22" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ TRADICIÓN NEIRA</t>
-        </is>
-      </c>
-      <c r="F22" s="7" t="n"/>
+          <t>DE SOL A SOL</t>
+        </is>
+      </c>
+      <c r="F22" s="7" t="inlineStr">
+        <is>
+          <t>EL ORGASMO DE LOS SAINOS</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="inlineStr">
@@ -1388,22 +1399,22 @@
       </c>
       <c r="B23" s="5" t="inlineStr">
         <is>
-          <t>Cita 4</t>
+          <t>Cita 5</t>
         </is>
       </c>
       <c r="C23" s="6" t="inlineStr">
         <is>
-          <t>CAFÉ MOLINA</t>
+          <t>REGIONAL S.A.S</t>
         </is>
       </c>
       <c r="D23" s="7" t="inlineStr">
         <is>
-          <t>EL ORGASMO DE LOS SAINOS</t>
+          <t>CAFÉ VALLE DE LIRIO</t>
         </is>
       </c>
       <c r="E23" s="7" t="inlineStr">
         <is>
-          <t>DELUXE COFFEE</t>
+          <t>CAFE FINCA MI TERRON</t>
         </is>
       </c>
       <c r="F23" s="7" t="n"/>
@@ -1416,22 +1427,22 @@
       </c>
       <c r="B24" s="5" t="inlineStr">
         <is>
-          <t>Cita 5</t>
+          <t>Cita 6</t>
         </is>
       </c>
       <c r="C24" s="6" t="inlineStr">
         <is>
-          <t>COLFRESH COFFEE</t>
+          <t>INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="D24" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ ERMITAÑO</t>
+          <t>CAFÉ MURAL</t>
         </is>
       </c>
       <c r="E24" s="7" t="inlineStr">
         <is>
-          <t>RUNA COFFEE</t>
+          <t>DON HEBER CAFÉ</t>
         </is>
       </c>
       <c r="F24" s="7" t="n"/>
@@ -1439,27 +1450,27 @@
     <row r="25">
       <c r="A25" s="5" t="inlineStr">
         <is>
-          <t>09:00 - 09:15</t>
+          <t>09:15 - 09:30</t>
         </is>
       </c>
       <c r="B25" s="5" t="inlineStr">
         <is>
-          <t>Cita 6</t>
+          <t>Cita 1</t>
         </is>
       </c>
       <c r="C25" s="6" t="inlineStr">
         <is>
-          <t>REGIONAL S.A.S</t>
+          <t>BOX BRAND</t>
         </is>
       </c>
       <c r="D25" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ VALLE DE LIRIO</t>
+          <t>RUNA COFFEE</t>
         </is>
       </c>
       <c r="E25" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ AGUA VIVA</t>
+          <t>CAFE FINCA MI TERRON</t>
         </is>
       </c>
       <c r="F25" s="7" t="n"/>
@@ -1467,55 +1478,59 @@
     <row r="26">
       <c r="A26" s="5" t="inlineStr">
         <is>
-          <t>09:00 - 09:15</t>
+          <t>09:15 - 09:30</t>
         </is>
       </c>
       <c r="B26" s="5" t="inlineStr">
         <is>
-          <t>Cita 7</t>
+          <t>Cita 2</t>
         </is>
       </c>
       <c r="C26" s="6" t="inlineStr">
         <is>
-          <t>ARMANDO VELÁSQUEZ</t>
+          <t>INMERSSO BOUTIQUE</t>
         </is>
       </c>
       <c r="D26" s="7" t="inlineStr">
         <is>
-          <t>LADERAS DEL TAPIAS</t>
+          <t>DELUXE COFFEE</t>
         </is>
       </c>
       <c r="E26" s="7" t="inlineStr">
         <is>
-          <t>DE SOL A SOL</t>
-        </is>
-      </c>
-      <c r="F26" s="7" t="n"/>
+          <t>FINCA LA FEDERICA</t>
+        </is>
+      </c>
+      <c r="F26" s="7" t="inlineStr">
+        <is>
+          <t>CAFÉ TRADICIÓN NEIRA</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="inlineStr">
         <is>
-          <t>09:00 - 09:15</t>
+          <t>09:15 - 09:30</t>
         </is>
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
-          <t>Cita 8</t>
+          <t>Cita 3</t>
         </is>
       </c>
       <c r="C27" s="6" t="inlineStr">
         <is>
-          <t>FLOR A FRUTO</t>
+          <t>REGIONAL S.A.S</t>
         </is>
       </c>
       <c r="D27" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ CAMPOHERMOSO</t>
+          <t>FINCA LA RIVERA</t>
         </is>
       </c>
       <c r="E27" s="7" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA</t>
+          <t>CAFÉ AGUA VIVA</t>
         </is>
       </c>
       <c r="F27" s="7" t="n"/>
@@ -1528,22 +1543,22 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
-          <t>Cita 1</t>
+          <t>Cita 4</t>
         </is>
       </c>
       <c r="C28" s="6" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS</t>
+          <t>FLOR A FRUTO</t>
         </is>
       </c>
       <c r="D28" s="7" t="inlineStr">
         <is>
-          <t>SANTA CRUZ DE LAS AGUAS</t>
+          <t>CAFÉ VALLE DE LIRIO</t>
         </is>
       </c>
       <c r="E28" s="7" t="inlineStr">
         <is>
-          <t>LADERAS DEL TAPIAS</t>
+          <t>DE SOL A SOL</t>
         </is>
       </c>
       <c r="F28" s="7" t="n"/>
@@ -1556,114 +1571,118 @@
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>Cita 2</t>
+          <t>Cita 5</t>
         </is>
       </c>
       <c r="C29" s="6" t="inlineStr">
         <is>
-          <t>BOX BRAND</t>
+          <t>INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="D29" s="7" t="inlineStr">
         <is>
-          <t>CAFE FINCA MI TERRON</t>
+          <t>SIETE LEONES CAFÉ</t>
         </is>
       </c>
       <c r="E29" s="7" t="inlineStr">
         <is>
-          <t>DON HEBER CAFÉ</t>
+          <t>LA PATRONA</t>
         </is>
       </c>
       <c r="F29" s="7" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA</t>
+          <t>CAFE MIS TAITAS</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="inlineStr">
         <is>
-          <t>09:15 - 09:30</t>
+          <t>09:30 - 09:45</t>
         </is>
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>Cita 3</t>
+          <t>Cita 1</t>
         </is>
       </c>
       <c r="C30" s="6" t="inlineStr">
         <is>
-          <t>INMERSSO BOUTIQUE</t>
+          <t>BOX BRAND</t>
         </is>
       </c>
       <c r="D30" s="7" t="inlineStr">
         <is>
-          <t>DELUXE COFFEE</t>
+          <t>CAFÉ VALLE DE LIRIO</t>
         </is>
       </c>
       <c r="E30" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ VALLE DE LIRIO</t>
+          <t>FINCA EL CASCABEL</t>
         </is>
       </c>
       <c r="F30" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ MURAL</t>
+          <t>FINCA LA RIVERA</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="inlineStr">
         <is>
-          <t>09:15 - 09:30</t>
+          <t>09:30 - 09:45</t>
         </is>
       </c>
       <c r="B31" s="5" t="inlineStr">
         <is>
-          <t>Cita 4</t>
+          <t>Cita 2</t>
         </is>
       </c>
       <c r="C31" s="6" t="inlineStr">
         <is>
-          <t>CAFÉ MOLINA</t>
+          <t>INMERSSO BOUTIQUE</t>
         </is>
       </c>
       <c r="D31" s="7" t="inlineStr">
         <is>
-          <t>RUNA COFFEE</t>
+          <t>DON HEBER CAFÉ</t>
         </is>
       </c>
       <c r="E31" s="7" t="inlineStr">
         <is>
-          <t>ROJO PASIÓN</t>
-        </is>
-      </c>
-      <c r="F31" s="7" t="n"/>
+          <t>LADERAS DEL TAPIAS</t>
+        </is>
+      </c>
+      <c r="F31" s="7" t="inlineStr">
+        <is>
+          <t>CAFÉ MURAL</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="inlineStr">
         <is>
-          <t>09:15 - 09:30</t>
+          <t>09:30 - 09:45</t>
         </is>
       </c>
       <c r="B32" s="5" t="inlineStr">
         <is>
-          <t>Cita 5</t>
+          <t>Cita 3</t>
         </is>
       </c>
       <c r="C32" s="6" t="inlineStr">
         <is>
-          <t>ARMANDO VELÁSQUEZ</t>
+          <t>CAFÉ MOLINA</t>
         </is>
       </c>
       <c r="D32" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ MATILDE 1960</t>
+          <t>EL ORGASMO DE LOS SAINOS</t>
         </is>
       </c>
       <c r="E32" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ AGUA VIVA</t>
+          <t>CAFE FINCA MI TERRON</t>
         </is>
       </c>
       <c r="F32" s="7" t="n"/>
@@ -1676,29 +1695,25 @@
       </c>
       <c r="B33" s="5" t="inlineStr">
         <is>
-          <t>Cita 1</t>
+          <t>Cita 4</t>
         </is>
       </c>
       <c r="C33" s="6" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS</t>
+          <t>COLFRESH COFFEE</t>
         </is>
       </c>
       <c r="D33" s="7" t="inlineStr">
         <is>
-          <t>SIETE LEONES CAFÉ</t>
+          <t>DELUXE COFFEE</t>
         </is>
       </c>
       <c r="E33" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ MURAL</t>
-        </is>
-      </c>
-      <c r="F33" s="7" t="inlineStr">
-        <is>
-          <t>CAFE ARTE</t>
-        </is>
-      </c>
+          <t>LA PATRONA</t>
+        </is>
+      </c>
+      <c r="F33" s="7" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="inlineStr">
@@ -1708,12 +1723,12 @@
       </c>
       <c r="B34" s="5" t="inlineStr">
         <is>
-          <t>Cita 2</t>
+          <t>Cita 5</t>
         </is>
       </c>
       <c r="C34" s="6" t="inlineStr">
         <is>
-          <t>BOX BRAND</t>
+          <t>REGIONAL S.A.S</t>
         </is>
       </c>
       <c r="D34" s="7" t="inlineStr">
@@ -1723,14 +1738,10 @@
       </c>
       <c r="E34" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ VALLE DE LIRIO</t>
-        </is>
-      </c>
-      <c r="F34" s="7" t="inlineStr">
-        <is>
           <t>ROJO PASIÓN</t>
         </is>
       </c>
+      <c r="F34" s="7" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="inlineStr">
@@ -1740,29 +1751,25 @@
       </c>
       <c r="B35" s="5" t="inlineStr">
         <is>
-          <t>Cita 3</t>
+          <t>Cita 6</t>
         </is>
       </c>
       <c r="C35" s="6" t="inlineStr">
         <is>
-          <t>INMERSSO BOUTIQUE</t>
+          <t>ARMANDO VELÁSQUEZ</t>
         </is>
       </c>
       <c r="D35" s="7" t="inlineStr">
         <is>
-          <t>RUNA COFFEE</t>
+          <t>FINCA LA FEDERICA</t>
         </is>
       </c>
       <c r="E35" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ MATILDE 1960</t>
-        </is>
-      </c>
-      <c r="F35" s="7" t="inlineStr">
-        <is>
-          <t>FINCA LA RIVERA</t>
-        </is>
-      </c>
+          <t>DE SOL A SOL</t>
+        </is>
+      </c>
+      <c r="F35" s="7" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="inlineStr">
@@ -1772,25 +1779,29 @@
       </c>
       <c r="B36" s="5" t="inlineStr">
         <is>
-          <t>Cita 4</t>
+          <t>Cita 7</t>
         </is>
       </c>
       <c r="C36" s="6" t="inlineStr">
         <is>
-          <t>REGIONAL S.A.S</t>
+          <t>INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="D36" s="7" t="inlineStr">
         <is>
-          <t>EL ORGASMO DE LOS SAINOS</t>
+          <t>CAFÉ TRADICIÓN NEIRA</t>
         </is>
       </c>
       <c r="E36" s="7" t="inlineStr">
         <is>
-          <t>DON HEBER CAFÉ</t>
-        </is>
-      </c>
-      <c r="F36" s="7" t="n"/>
+          <t>CAFE ARTE</t>
+        </is>
+      </c>
+      <c r="F36" s="7" t="inlineStr">
+        <is>
+          <t>D'CLEO COFFEE</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="inlineStr">
@@ -1805,22 +1816,22 @@
       </c>
       <c r="C37" s="6" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS</t>
+          <t>BOX BRAND</t>
         </is>
       </c>
       <c r="D37" s="7" t="inlineStr">
         <is>
-          <t>CAFE GRANEAO</t>
+          <t>SIETE LEONES CAFÉ</t>
         </is>
       </c>
       <c r="E37" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ MATILDE 1960</t>
+          <t>ROJO PASIÓN</t>
         </is>
       </c>
       <c r="F37" s="7" t="inlineStr">
         <is>
-          <t>DON HEBER CAFÉ</t>
+          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS</t>
         </is>
       </c>
     </row>
@@ -1837,22 +1848,22 @@
       </c>
       <c r="C38" s="6" t="inlineStr">
         <is>
-          <t>BOX BRAND</t>
+          <t>INMERSSO BOUTIQUE</t>
         </is>
       </c>
       <c r="D38" s="7" t="inlineStr">
         <is>
-          <t>FINCA EL CASCABEL</t>
+          <t>CAFÉ ERMITAÑO</t>
         </is>
       </c>
       <c r="E38" s="7" t="inlineStr">
         <is>
-          <t>DELUXE COFFEE</t>
+          <t>CAFÉ OASIS DE SAMDA</t>
         </is>
       </c>
       <c r="F38" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ MURAL</t>
+          <t>CAFÉ VALLE DE LIRIO</t>
         </is>
       </c>
     </row>
@@ -1869,17 +1880,17 @@
       </c>
       <c r="C39" s="6" t="inlineStr">
         <is>
-          <t>INMERSSO BOUTIQUE</t>
+          <t>CAFÉ MOLINA</t>
         </is>
       </c>
       <c r="D39" s="7" t="inlineStr">
         <is>
-          <t>LADERAS DEL TAPIAS</t>
+          <t>RUNA COFFEE</t>
         </is>
       </c>
       <c r="E39" s="7" t="inlineStr">
         <is>
-          <t>ROJO PASIÓN</t>
+          <t>FINCA LA RIVERA</t>
         </is>
       </c>
       <c r="F39" s="7" t="n"/>
@@ -1902,19 +1913,15 @@
       </c>
       <c r="D40" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ AGUA VIVA</t>
+          <t>CAFÉ MURAL</t>
         </is>
       </c>
       <c r="E40" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ VALLE DE LIRIO</t>
-        </is>
-      </c>
-      <c r="F40" s="7" t="inlineStr">
-        <is>
-          <t>CAFÉ ARENILLO</t>
-        </is>
-      </c>
+          <t>FINCA LA FEDERICA</t>
+        </is>
+      </c>
+      <c r="F40" s="7" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="inlineStr">
@@ -1929,48 +1936,56 @@
       </c>
       <c r="C41" s="6" t="inlineStr">
         <is>
-          <t>REGIONAL S.A.S</t>
+          <t>FLOR A FRUTO</t>
         </is>
       </c>
       <c r="D41" s="7" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA</t>
+          <t>CAFÉ AGUA VIVA</t>
         </is>
       </c>
       <c r="E41" s="7" t="inlineStr">
         <is>
-          <t>CAFE ARTE</t>
-        </is>
-      </c>
-      <c r="F41" s="7" t="n"/>
+          <t>CAFE FINCA MI TERRON</t>
+        </is>
+      </c>
+      <c r="F41" s="7" t="inlineStr">
+        <is>
+          <t>DELUXE COFFEE</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="inlineStr">
         <is>
-          <t>09:45 - 10:00</t>
+          <t>10:00 - 10:15</t>
         </is>
       </c>
       <c r="B42" s="5" t="inlineStr">
         <is>
-          <t>Cita 6</t>
+          <t>Cita 1</t>
         </is>
       </c>
       <c r="C42" s="6" t="inlineStr">
         <is>
-          <t>ARMANDO VELÁSQUEZ</t>
+          <t>BOX BRAND</t>
         </is>
       </c>
       <c r="D42" s="7" t="inlineStr">
         <is>
-          <t>RUNA COFFEE</t>
+          <t>CAFÉ GRANADA</t>
         </is>
       </c>
       <c r="E42" s="7" t="inlineStr">
         <is>
-          <t>CAFE FINCA MI TERRON</t>
-        </is>
-      </c>
-      <c r="F42" s="7" t="n"/>
+          <t>SANTA CRUZ DE LAS AGUAS</t>
+        </is>
+      </c>
+      <c r="F42" s="7" t="inlineStr">
+        <is>
+          <t>CAFÉ MATILDE 1960</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="inlineStr">
@@ -1980,27 +1995,27 @@
       </c>
       <c r="B43" s="5" t="inlineStr">
         <is>
-          <t>Cita 1</t>
+          <t>Cita 2</t>
         </is>
       </c>
       <c r="C43" s="6" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS</t>
+          <t>INMERSSO BOUTIQUE</t>
         </is>
       </c>
       <c r="D43" s="7" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA</t>
+          <t>CAFÉ AGUA VIVA</t>
         </is>
       </c>
       <c r="E43" s="7" t="inlineStr">
         <is>
-          <t>DELUXE COFFEE</t>
+          <t>CAFÉ ARENILLO</t>
         </is>
       </c>
       <c r="F43" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ ARENILLO</t>
+          <t>SIETE LEONES CAFÉ</t>
         </is>
       </c>
     </row>
@@ -2012,29 +2027,25 @@
       </c>
       <c r="B44" s="5" t="inlineStr">
         <is>
-          <t>Cita 2</t>
+          <t>Cita 3</t>
         </is>
       </c>
       <c r="C44" s="6" t="inlineStr">
         <is>
-          <t>BOX BRAND</t>
+          <t>COLFRESH COFFEE</t>
         </is>
       </c>
       <c r="D44" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ GRANADA</t>
+          <t>FINCA LA RIVERA</t>
         </is>
       </c>
       <c r="E44" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ AGUA VIVA</t>
-        </is>
-      </c>
-      <c r="F44" s="7" t="inlineStr">
-        <is>
-          <t>CAFÉ TRADICIÓN NEIRA</t>
-        </is>
-      </c>
+          <t>RUNA COFFEE</t>
+        </is>
+      </c>
+      <c r="F44" s="7" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="inlineStr">
@@ -2044,12 +2055,12 @@
       </c>
       <c r="B45" s="5" t="inlineStr">
         <is>
-          <t>Cita 3</t>
+          <t>Cita 4</t>
         </is>
       </c>
       <c r="C45" s="6" t="inlineStr">
         <is>
-          <t>FLOR A FRUTO</t>
+          <t>INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="D45" s="7" t="inlineStr">
@@ -2059,39 +2070,35 @@
       </c>
       <c r="E45" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ VALLE DE LIRIO</t>
-        </is>
-      </c>
-      <c r="F45" s="7" t="inlineStr">
-        <is>
-          <t>DE SOL A SOL</t>
-        </is>
-      </c>
+          <t>FINCA EL CASCABEL</t>
+        </is>
+      </c>
+      <c r="F45" s="7" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="5" t="inlineStr">
         <is>
-          <t>10:15 - 10:30</t>
+          <t>10:00 - 10:15</t>
         </is>
       </c>
       <c r="B46" s="5" t="inlineStr">
         <is>
-          <t>Cita 1</t>
+          <t>Cita 5</t>
         </is>
       </c>
       <c r="C46" s="6" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS</t>
+          <t>PROCOLOMBIA</t>
         </is>
       </c>
       <c r="D46" s="7" t="inlineStr">
         <is>
-          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS</t>
+          <t>CAFÉ VALLE DE LIRIO</t>
         </is>
       </c>
       <c r="E46" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ LA AVANZANTE</t>
+          <t>EL ORGASMO DE LOS SAINOS</t>
         </is>
       </c>
       <c r="F46" s="7" t="n"/>
@@ -2104,7 +2111,7 @@
       </c>
       <c r="B47" s="5" t="inlineStr">
         <is>
-          <t>Cita 2</t>
+          <t>Cita 1</t>
         </is>
       </c>
       <c r="C47" s="6" t="inlineStr">
@@ -2114,12 +2121,12 @@
       </c>
       <c r="D47" s="7" t="inlineStr">
         <is>
-          <t>SIETE LEONES CAFÉ</t>
+          <t>CAFÉ ARENILLO</t>
         </is>
       </c>
       <c r="E47" s="7" t="inlineStr">
         <is>
-          <t>CAFE ARTE</t>
+          <t>EL ORGASMO DE LOS SAINOS</t>
         </is>
       </c>
       <c r="F47" s="7" t="n"/>
@@ -2132,7 +2139,7 @@
       </c>
       <c r="B48" s="5" t="inlineStr">
         <is>
-          <t>Cita 3</t>
+          <t>Cita 2</t>
         </is>
       </c>
       <c r="C48" s="6" t="inlineStr">
@@ -2142,12 +2149,12 @@
       </c>
       <c r="D48" s="7" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA</t>
+          <t>CAFÉ LA AVANZANTE</t>
         </is>
       </c>
       <c r="E48" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ AGUA VIVA</t>
+          <t>RUNA COFFEE</t>
         </is>
       </c>
       <c r="F48" s="7" t="n"/>
@@ -2160,22 +2167,22 @@
       </c>
       <c r="B49" s="5" t="inlineStr">
         <is>
-          <t>Cita 4</t>
+          <t>Cita 3</t>
         </is>
       </c>
       <c r="C49" s="6" t="inlineStr">
         <is>
-          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
+          <t>FLOR A FRUTO</t>
         </is>
       </c>
       <c r="D49" s="7" t="inlineStr">
         <is>
-          <t>ROJO PASIÓN</t>
+          <t>FINCA LA RIVERA</t>
         </is>
       </c>
       <c r="E49" s="7" t="inlineStr">
         <is>
-          <t>FINCA EL CASCABEL</t>
+          <t>CAFÉ ERMITAÑO</t>
         </is>
       </c>
       <c r="F49" s="7" t="n"/>
@@ -2188,22 +2195,22 @@
       </c>
       <c r="B50" s="5" t="inlineStr">
         <is>
-          <t>Cita 5</t>
+          <t>Cita 4</t>
         </is>
       </c>
       <c r="C50" s="6" t="inlineStr">
         <is>
-          <t>FLOR A FRUTO</t>
+          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
         </is>
       </c>
       <c r="D50" s="7" t="inlineStr">
         <is>
-          <t>RUNA COFFEE</t>
+          <t>ROJO PASIÓN</t>
         </is>
       </c>
       <c r="E50" s="7" t="inlineStr">
         <is>
-          <t>DELUXE COFFEE</t>
+          <t>FINCA EL CASCABEL</t>
         </is>
       </c>
       <c r="F50" s="7" t="n"/>
@@ -2211,62 +2218,66 @@
     <row r="51">
       <c r="A51" s="5" t="inlineStr">
         <is>
-          <t>10:30 - 10:45</t>
+          <t>10:15 - 10:30</t>
         </is>
       </c>
       <c r="B51" s="5" t="inlineStr">
         <is>
-          <t>Cita 1</t>
+          <t>Cita 5</t>
         </is>
       </c>
       <c r="C51" s="6" t="inlineStr">
         <is>
-          <t>INMERSSO BOUTIQUE</t>
+          <t>ARMANDO VELÁSQUEZ</t>
         </is>
       </c>
       <c r="D51" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ ARENILLO</t>
+          <t>DELUXE COFFEE</t>
         </is>
       </c>
       <c r="E51" s="7" t="inlineStr">
         <is>
-          <t>SIETE LEONES CAFÉ</t>
+          <t>CAFÉ AGUA VIVA</t>
         </is>
       </c>
       <c r="F51" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ OASIS DE SAMDA</t>
+          <t>CAFÉ MATILDE 1960</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="inlineStr">
         <is>
-          <t>10:30 - 10:45</t>
+          <t>10:15 - 10:30</t>
         </is>
       </c>
       <c r="B52" s="5" t="inlineStr">
         <is>
-          <t>Cita 2</t>
+          <t>Cita 6</t>
         </is>
       </c>
       <c r="C52" s="6" t="inlineStr">
         <is>
-          <t>NEIRA YORK COFFEE</t>
+          <t>INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="D52" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ CAMPOHERMOSO</t>
+          <t>SANTA CRUZ DE LAS AGUAS</t>
         </is>
       </c>
       <c r="E52" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ LA AVANZANTE</t>
-        </is>
-      </c>
-      <c r="F52" s="7" t="n"/>
+          <t>CAFÉ VALLE DE LIRIO</t>
+        </is>
+      </c>
+      <c r="F52" s="7" t="inlineStr">
+        <is>
+          <t>CAFE GRANEAO</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="inlineStr">
@@ -2276,22 +2287,22 @@
       </c>
       <c r="B53" s="5" t="inlineStr">
         <is>
-          <t>Cita 3</t>
+          <t>Cita 1</t>
         </is>
       </c>
       <c r="C53" s="6" t="inlineStr">
         <is>
-          <t>COLFRESH COFFEE</t>
+          <t>NEIRA YORK COFFEE</t>
         </is>
       </c>
       <c r="D53" s="7" t="inlineStr">
         <is>
+          <t>CINCO DAMAS</t>
+        </is>
+      </c>
+      <c r="E53" s="7" t="inlineStr">
+        <is>
           <t>FINCA LA RIVERA</t>
-        </is>
-      </c>
-      <c r="E53" s="7" t="inlineStr">
-        <is>
-          <t>DELUXE COFFEE</t>
         </is>
       </c>
       <c r="F53" s="7" t="n"/>
@@ -2304,22 +2315,22 @@
       </c>
       <c r="B54" s="5" t="inlineStr">
         <is>
-          <t>Cita 4</t>
+          <t>Cita 2</t>
         </is>
       </c>
       <c r="C54" s="6" t="inlineStr">
         <is>
-          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
+          <t>FLOR A FRUTO</t>
         </is>
       </c>
       <c r="D54" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ MATILDE 1960</t>
+          <t>SANTA CRUZ DE LAS AGUAS</t>
         </is>
       </c>
       <c r="E54" s="7" t="inlineStr">
         <is>
-          <t>RUNA COFFEE</t>
+          <t>ROJO PASIÓN</t>
         </is>
       </c>
       <c r="F54" s="7" t="n"/>
@@ -2327,22 +2338,22 @@
     <row r="55">
       <c r="A55" s="5" t="inlineStr">
         <is>
-          <t>10:45 - 11:00</t>
+          <t>10:30 - 10:45</t>
         </is>
       </c>
       <c r="B55" s="5" t="inlineStr">
         <is>
-          <t>Cita 1</t>
+          <t>Cita 3</t>
         </is>
       </c>
       <c r="C55" s="6" t="inlineStr">
         <is>
-          <t>NEIRA YORK COFFEE</t>
+          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
         </is>
       </c>
       <c r="D55" s="7" t="inlineStr">
         <is>
-          <t>CINCO DAMAS</t>
+          <t>CAFÉ OASIS DE SAMDA</t>
         </is>
       </c>
       <c r="E55" s="7" t="inlineStr">
@@ -2355,30 +2366,34 @@
     <row r="56">
       <c r="A56" s="5" t="inlineStr">
         <is>
-          <t>10:45 - 11:00</t>
+          <t>10:30 - 10:45</t>
         </is>
       </c>
       <c r="B56" s="5" t="inlineStr">
         <is>
-          <t>Cita 2</t>
+          <t>Cita 4</t>
         </is>
       </c>
       <c r="C56" s="6" t="inlineStr">
         <is>
-          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
+          <t>INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="D56" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ TRADICIÓN NEIRA</t>
+          <t>FINCA LA FEDERICA</t>
         </is>
       </c>
       <c r="E56" s="7" t="inlineStr">
         <is>
-          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS</t>
-        </is>
-      </c>
-      <c r="F56" s="7" t="n"/>
+          <t>DELUXE COFFEE</t>
+        </is>
+      </c>
+      <c r="F56" s="7" t="inlineStr">
+        <is>
+          <t>CAFÉ MATILDE 1960</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="inlineStr">
@@ -2388,54 +2403,50 @@
       </c>
       <c r="B57" s="5" t="inlineStr">
         <is>
-          <t>Cita 3</t>
+          <t>Cita 1</t>
         </is>
       </c>
       <c r="C57" s="6" t="inlineStr">
         <is>
-          <t>FLOR A FRUTO</t>
+          <t>NEIRA YORK COFFEE</t>
         </is>
       </c>
       <c r="D57" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ OASIS DE SAMDA</t>
+          <t>ROJO PASIÓN</t>
         </is>
       </c>
       <c r="E57" s="7" t="inlineStr">
         <is>
-          <t>FINCA EL CASCABEL</t>
-        </is>
-      </c>
-      <c r="F57" s="7" t="inlineStr">
-        <is>
-          <t>ROJO PASIÓN</t>
-        </is>
-      </c>
+          <t>CAFÉ CAMPOHERMOSO</t>
+        </is>
+      </c>
+      <c r="F57" s="7" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="inlineStr">
         <is>
-          <t>11:00 - 11:15</t>
+          <t>10:45 - 11:00</t>
         </is>
       </c>
       <c r="B58" s="5" t="inlineStr">
         <is>
-          <t>Cita 1</t>
+          <t>Cita 2</t>
         </is>
       </c>
       <c r="C58" s="6" t="inlineStr">
         <is>
-          <t>NEIRA YORK COFFEE</t>
+          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
         </is>
       </c>
       <c r="D58" s="7" t="inlineStr">
         <is>
-          <t>ROJO PASIÓN</t>
+          <t>FINCA LA FEDERICA</t>
         </is>
       </c>
       <c r="E58" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ VALLE DE LIRIO</t>
+          <t>CAFÉ TRADICIÓN NEIRA</t>
         </is>
       </c>
       <c r="F58" s="7" t="n"/>
@@ -2443,27 +2454,27 @@
     <row r="59">
       <c r="A59" s="5" t="inlineStr">
         <is>
-          <t>11:00 - 11:15</t>
+          <t>10:45 - 11:00</t>
         </is>
       </c>
       <c r="B59" s="5" t="inlineStr">
         <is>
-          <t>Cita 2</t>
+          <t>Cita 3</t>
         </is>
       </c>
       <c r="C59" s="6" t="inlineStr">
         <is>
-          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
+          <t>ARMANDO VELÁSQUEZ</t>
         </is>
       </c>
       <c r="D59" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ AGUA VIVA</t>
+          <t>RUNA COFFEE</t>
         </is>
       </c>
       <c r="E59" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ OASIS DE SAMDA</t>
+          <t>CAFÉ VALLE DE LIRIO</t>
         </is>
       </c>
       <c r="F59" s="7" t="n"/>
@@ -2471,7 +2482,7 @@
     <row r="60">
       <c r="A60" s="5" t="inlineStr">
         <is>
-          <t>11:15 - 11:30</t>
+          <t>11:00 - 11:15</t>
         </is>
       </c>
       <c r="B60" s="5" t="inlineStr">
@@ -2481,29 +2492,25 @@
       </c>
       <c r="C60" s="6" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS</t>
+          <t>NEIRA YORK COFFEE</t>
         </is>
       </c>
       <c r="D60" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ AGUA VIVA</t>
+          <t>CAFÉ MURAL</t>
         </is>
       </c>
       <c r="E60" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ ORIGEN DE LA MONTAÑA</t>
-        </is>
-      </c>
-      <c r="F60" s="7" t="inlineStr">
-        <is>
           <t>CAFÉ VALLE DE LIRIO</t>
         </is>
       </c>
+      <c r="F60" s="7" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="inlineStr">
         <is>
-          <t>11:15 - 11:30</t>
+          <t>11:00 - 11:15</t>
         </is>
       </c>
       <c r="B61" s="5" t="inlineStr">
@@ -2513,17 +2520,17 @@
       </c>
       <c r="C61" s="6" t="inlineStr">
         <is>
-          <t>NEIRA YORK COFFEE</t>
+          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
         </is>
       </c>
       <c r="D61" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ MURAL</t>
+          <t>CAFÉ AGUA VIVA</t>
         </is>
       </c>
       <c r="E61" s="7" t="inlineStr">
         <is>
-          <t>DE SOL A SOL</t>
+          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS</t>
         </is>
       </c>
       <c r="F61" s="7" t="n"/>
@@ -2531,7 +2538,7 @@
     <row r="62">
       <c r="A62" s="5" t="inlineStr">
         <is>
-          <t>11:30 - 11:45</t>
+          <t>11:15 - 11:30</t>
         </is>
       </c>
       <c r="B62" s="5" t="inlineStr">
@@ -2546,20 +2553,24 @@
       </c>
       <c r="D62" s="7" t="inlineStr">
         <is>
-          <t>CAFÉ ARENILLO</t>
+          <t>CAFÉ AGUA VIVA</t>
         </is>
       </c>
       <c r="E62" s="7" t="inlineStr">
         <is>
+          <t>DON HEBER CAFÉ</t>
+        </is>
+      </c>
+      <c r="F62" s="7" t="inlineStr">
+        <is>
           <t>CAFÉ ORIGEN DE LA MONTAÑA</t>
         </is>
       </c>
-      <c r="F62" s="7" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="inlineStr">
         <is>
-          <t>11:45 - 12:00</t>
+          <t>11:30 - 11:45</t>
         </is>
       </c>
       <c r="B63" s="5" t="inlineStr">
@@ -2574,12 +2585,12 @@
       </c>
       <c r="D63" s="7" t="inlineStr">
         <is>
+          <t>CAFÉ MATILDE 1960</t>
+        </is>
+      </c>
+      <c r="E63" s="7" t="inlineStr">
+        <is>
           <t>CAFÉ ORIGEN DE LA MONTAÑA</t>
-        </is>
-      </c>
-      <c r="E63" s="7" t="inlineStr">
-        <is>
-          <t>CAFÉ AGUA VIVA</t>
         </is>
       </c>
       <c r="F63" s="7" t="n"/>
@@ -2587,30 +2598,90 @@
     <row r="64">
       <c r="A64" s="5" t="inlineStr">
         <is>
+          <t>11:30 - 11:45</t>
+        </is>
+      </c>
+      <c r="B64" s="5" t="inlineStr">
+        <is>
+          <t>Cita 2</t>
+        </is>
+      </c>
+      <c r="C64" s="6" t="inlineStr">
+        <is>
+          <t>NEIRA YORK COFFEE</t>
+        </is>
+      </c>
+      <c r="D64" s="7" t="inlineStr">
+        <is>
+          <t>DE SOL A SOL</t>
+        </is>
+      </c>
+      <c r="E64" s="7" t="inlineStr">
+        <is>
+          <t>CAFÉ AGUA VIVA</t>
+        </is>
+      </c>
+      <c r="F64" s="7" t="n"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="5" t="inlineStr">
+        <is>
+          <t>11:45 - 12:00</t>
+        </is>
+      </c>
+      <c r="B65" s="5" t="inlineStr">
+        <is>
+          <t>Cita 1</t>
+        </is>
+      </c>
+      <c r="C65" s="6" t="inlineStr">
+        <is>
+          <t>INTERLINK2AMERICAS</t>
+        </is>
+      </c>
+      <c r="D65" s="7" t="inlineStr">
+        <is>
+          <t>CAFÉ ORIGEN DE LA MONTAÑA</t>
+        </is>
+      </c>
+      <c r="E65" s="7" t="inlineStr">
+        <is>
+          <t>FINCA LA RIVERA</t>
+        </is>
+      </c>
+      <c r="F65" s="7" t="inlineStr">
+        <is>
+          <t>LADERAS DEL TAPIAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="5" t="inlineStr">
+        <is>
           <t>12:00 - 12:15</t>
         </is>
       </c>
-      <c r="B64" s="5" t="inlineStr">
+      <c r="B66" s="5" t="inlineStr">
         <is>
           <t>Cita 1</t>
         </is>
       </c>
-      <c r="C64" s="6" t="inlineStr">
+      <c r="C66" s="6" t="inlineStr">
         <is>
           <t>PROCOLOMBIA</t>
         </is>
       </c>
-      <c r="D64" s="7" t="inlineStr">
+      <c r="D66" s="7" t="inlineStr">
         <is>
           <t>CAFÉ ORIGEN DE LA MONTAÑA</t>
         </is>
       </c>
-      <c r="E64" s="7" t="inlineStr">
-        <is>
-          <t>CAFÉ VALLE DE LIRIO</t>
-        </is>
-      </c>
-      <c r="F64" s="7" t="n"/>
+      <c r="E66" s="7" t="inlineStr">
+        <is>
+          <t>D'CLEO COFFEE</t>
+        </is>
+      </c>
+      <c r="F66" s="7" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2623,7 +2694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2668,357 +2739,357 @@
     <row r="2">
       <c r="A2" s="5" t="inlineStr">
         <is>
-          <t>CAFE ARTE</t>
+          <t>CAFE FINCA MI TERRON</t>
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>4/4</t>
         </is>
       </c>
       <c r="D2" s="5" t="inlineStr">
         <is>
-          <t>PROCOLOMBIA; INTERLINK2AMERICAS; REGIONAL S.A.S; BOX BRAND</t>
+          <t>PROCOLOMBIA; ARMANDO VELÁSQUEZ; REGIONAL S.A.S; BOX BRAND; CAFÉ MOLINA; FLOR A FRUTO; INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="E2" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 09:30 - 09:45; 09:45 - 10:00; 10:15 - 10:30</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:00 - 10:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ LA AVANZANTE</t>
+          <t>EL ORGASMO DE LOS SAINOS</t>
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>3/3</t>
         </is>
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>PROCOLOMBIA; INMERSSO BOUTIQUE; INTERLINK2AMERICAS; NEIRA YORK COFFEE</t>
+          <t>REGIONAL S.A.S; COLFRESH COFFEE; CAFÉ MOLINA; PROCOLOMBIA; BOX BRAND</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 09:00 - 09:15; 10:15 - 10:30; 10:30 - 10:45</t>
+          <t>08:30 - 08:45; 09:00 - 09:15; 09:30 - 09:45; 10:00 - 10:15; 10:15 - 10:30</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>EL ORGASMO DE LOS SAINOS</t>
+          <t>CAFÉ ARENILLO</t>
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>5/5</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>COLFRESH COFFEE; PROCOLOMBIA; CAFÉ MOLINA; REGIONAL S.A.S</t>
+          <t>INTERLINK2AMERICAS; FLOR A FRUTO; COLFRESH COFFEE; INMERSSO BOUTIQUE; BOX BRAND</t>
         </is>
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:30 - 09:45</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 10:00 - 10:15; 10:15 - 10:30</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>LADERAS DEL TAPIAS</t>
+          <t>SANTA CRUZ DE LAS AGUAS</t>
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>3/3</t>
         </is>
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>BOX BRAND; ARMANDO VELÁSQUEZ; INTERLINK2AMERICAS; INMERSSO BOUTIQUE</t>
+          <t>BOX BRAND; INTERLINK2AMERICAS; FLOR A FRUTO</t>
         </is>
       </c>
       <c r="E5" s="5" t="inlineStr">
         <is>
-          <t>08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:45 - 10:00</t>
+          <t>10:00 - 10:15; 10:15 - 10:30; 10:30 - 10:45</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>LA PATRONA</t>
+          <t>DON HEBER CAFÉ</t>
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>5/5</t>
         </is>
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
-          <t>COLFRESH COFFEE; INTERLINK2AMERICAS</t>
+          <t>REGIONAL S.A.S; ARMANDO VELÁSQUEZ; INTERLINK2AMERICAS; INMERSSO BOUTIQUE; BOX BRAND</t>
         </is>
       </c>
       <c r="E6" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:30 - 09:45; 11:15 - 11:30</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
         <is>
-          <t>CAFE MIS TAITAS</t>
+          <t>CAFÉ TRADICIÓN NEIRA</t>
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>1/1</t>
+          <t>4/4</t>
         </is>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS</t>
+          <t>BOX BRAND; INMERSSO BOUTIQUE; INTERLINK2AMERICAS; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45</t>
+          <t>08:45 - 09:00; 09:15 - 09:30; 09:30 - 09:45; 10:45 - 11:00</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>FINCA EL CASCABEL</t>
+          <t>CAFÉ OASIS DE SAMDA</t>
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>5/5</t>
+          <t>3/3</t>
         </is>
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>ARMANDO VELÁSQUEZ; INTERLINK2AMERICAS; BOX BRAND; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.; FLOR A FRUTO</t>
+          <t>FLOR A FRUTO; INMERSSO BOUTIQUE; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
         </is>
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:45 - 10:00; 10:15 - 10:30; 10:45 - 11:00</t>
+          <t>08:30 - 08:45; 09:45 - 10:00; 10:30 - 10:45</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t>CAFE FINCA MI TERRON</t>
+          <t>LA PATRONA</t>
         </is>
       </c>
       <c r="B9" s="5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>2/2</t>
         </is>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS; BOX BRAND; ARMANDO VELÁSQUEZ; FLOR A FRUTO</t>
+          <t>INTERLINK2AMERICAS; COLFRESH COFFEE</t>
         </is>
       </c>
       <c r="E9" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 09:15 - 09:30; 09:45 - 10:00; 10:00 - 10:15</t>
+          <t>09:15 - 09:30; 09:30 - 09:45</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ ORIGEN DE LA MONTAÑA</t>
+          <t>FINCA EL CASCABEL</t>
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>5/5</t>
         </is>
       </c>
       <c r="D10" s="5" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS; BOX BRAND; INMERSSO BOUTIQUE; PROCOLOMBIA</t>
+          <t>ARMANDO VELÁSQUEZ; FLOR A FRUTO; BOX BRAND; INTERLINK2AMERICAS; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
         </is>
       </c>
       <c r="E10" s="5" t="inlineStr">
         <is>
-          <t>11:15 - 11:30; 11:30 - 11:45; 11:45 - 12:00; 12:00 - 12:15</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:30 - 09:45; 10:00 - 10:15; 10:15 - 10:30</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="inlineStr">
         <is>
-          <t>DELUXE COFFEE</t>
+          <t>CAFÉ ERMITAÑO</t>
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>8/8</t>
+          <t>3/3</t>
         </is>
       </c>
       <c r="D11" s="5" t="inlineStr">
         <is>
-          <t>REGIONAL S.A.S; ARMANDO VELÁSQUEZ; CAFÉ MOLINA; INMERSSO BOUTIQUE; BOX BRAND; INTERLINK2AMERICAS; FLOR A FRUTO; COLFRESH COFFEE</t>
+          <t>COLFRESH COFFEE; INMERSSO BOUTIQUE; FLOR A FRUTO</t>
         </is>
       </c>
       <c r="E11" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:45 - 10:00; 10:00 - 10:15; 10:15 - 10:30; 10:30 - 10:45</t>
+          <t>08:30 - 08:45; 09:45 - 10:00; 10:15 - 10:30</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ GRANADA</t>
+          <t>DELUXE COFFEE</t>
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C12" s="5" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>8/8</t>
         </is>
       </c>
       <c r="D12" s="5" t="inlineStr">
         <is>
-          <t>INMERSSO BOUTIQUE; INTERLINK2AMERICAS; BOX BRAND</t>
+          <t>REGIONAL S.A.S; CAFÉ MOLINA; BOX BRAND; INMERSSO BOUTIQUE; COLFRESH COFFEE; FLOR A FRUTO; ARMANDO VELÁSQUEZ; INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="E12" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 09:00 - 09:15; 10:00 - 10:15</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:15 - 10:30; 10:30 - 10:45</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ TRADICIÓN NEIRA</t>
+          <t>RUNA COFFEE</t>
         </is>
       </c>
       <c r="B13" s="5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>8/8</t>
         </is>
       </c>
       <c r="D13" s="5" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS; INMERSSO BOUTIQUE; BOX BRAND; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
+          <t>FLOR A FRUTO; INMERSSO BOUTIQUE; BOX BRAND; CAFÉ MOLINA; COLFRESH COFFEE; NEIRA YORK COFFEE; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.; ARMANDO VELÁSQUEZ</t>
         </is>
       </c>
       <c r="E13" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 09:00 - 09:15; 10:00 - 10:15; 10:45 - 11:00</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:15 - 09:30; 09:45 - 10:00; 10:00 - 10:15; 10:15 - 10:30; 10:30 - 10:45; 10:45 - 11:00</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ ARENILLO</t>
+          <t>CAFE GRANEAO</t>
         </is>
       </c>
       <c r="B14" s="5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>5/5</t>
+          <t>1/1</t>
         </is>
       </c>
       <c r="D14" s="5" t="inlineStr">
         <is>
-          <t>FLOR A FRUTO; COLFRESH COFFEE; INTERLINK2AMERICAS; INMERSSO BOUTIQUE; BOX BRAND</t>
+          <t>INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="E14" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 09:45 - 10:00; 10:00 - 10:15; 10:30 - 10:45; 11:30 - 11:45</t>
+          <t>10:15 - 10:30</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>D'CLEO COFFEE</t>
+          <t>CAFÉ VALLE DE LIRIO</t>
         </is>
       </c>
       <c r="B15" s="5" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>10/10</t>
         </is>
       </c>
       <c r="D15" s="5" t="inlineStr">
         <is>
-          <t>BOX BRAND; PROCOLOMBIA; INTERLINK2AMERICAS</t>
+          <t>CAFÉ MOLINA; COLFRESH COFFEE; REGIONAL S.A.S; FLOR A FRUTO; BOX BRAND; INMERSSO BOUTIQUE; PROCOLOMBIA; INTERLINK2AMERICAS; ARMANDO VELÁSQUEZ; NEIRA YORK COFFEE</t>
         </is>
       </c>
       <c r="E15" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:00 - 10:15; 10:15 - 10:30; 10:45 - 11:00; 11:00 - 11:15</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="inlineStr">
         <is>
-          <t>CINCO DAMAS</t>
+          <t>CAFÉ GRANADA</t>
         </is>
       </c>
       <c r="B16" s="5" t="n">
@@ -3031,169 +3102,169 @@
       </c>
       <c r="D16" s="5" t="inlineStr">
         <is>
-          <t>ARMANDO VELÁSQUEZ; INMERSSO BOUTIQUE; NEIRA YORK COFFEE</t>
+          <t>INMERSSO BOUTIQUE; INTERLINK2AMERICAS; BOX BRAND</t>
         </is>
       </c>
       <c r="E16" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 10:45 - 11:00</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 10:00 - 10:15</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA</t>
+          <t>CAFÉ MATILDE 1960</t>
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
-          <t>9/9</t>
+          <t>6/7</t>
         </is>
       </c>
       <c r="D17" s="5" t="inlineStr">
         <is>
-          <t>PROCOLOMBIA; CAFÉ MOLINA; FLOR A FRUTO; BOX BRAND; INMERSSO BOUTIQUE; REGIONAL S.A.S; INTERLINK2AMERICAS; NEIRA YORK COFFEE; COLFRESH COFFEE</t>
+          <t>COLFRESH COFFEE; REGIONAL S.A.S; BOX BRAND; ARMANDO VELÁSQUEZ; INTERLINK2AMERICAS; INMERSSO BOUTIQUE</t>
         </is>
       </c>
       <c r="E17" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:00 - 10:15; 10:15 - 10:30; 10:30 - 10:45</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 10:00 - 10:15; 10:15 - 10:30; 10:30 - 10:45; 11:30 - 11:45</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="inlineStr">
         <is>
-          <t>DE SOL A SOL</t>
+          <t>CINCO DAMAS</t>
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>5/5</t>
+          <t>3/3</t>
         </is>
       </c>
       <c r="D18" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ MOLINA; COLFRESH COFFEE; ARMANDO VELÁSQUEZ; FLOR A FRUTO; NEIRA YORK COFFEE</t>
+          <t>ARMANDO VELÁSQUEZ; INMERSSO BOUTIQUE; NEIRA YORK COFFEE</t>
         </is>
       </c>
       <c r="E18" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 10:00 - 10:15; 11:15 - 11:30</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 10:30 - 10:45</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>SANTA CRUZ DE LAS AGUAS</t>
+          <t>FINCA LA RIVERA</t>
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>9/9</t>
         </is>
       </c>
       <c r="D19" s="5" t="inlineStr">
         <is>
-          <t>FLOR A FRUTO; BOX BRAND; INTERLINK2AMERICAS</t>
+          <t>PROCOLOMBIA; INMERSSO BOUTIQUE; REGIONAL S.A.S; BOX BRAND; CAFÉ MOLINA; COLFRESH COFFEE; FLOR A FRUTO; NEIRA YORK COFFEE; INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="E19" s="5" t="inlineStr">
         <is>
-          <t>08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30</t>
+          <t>08:30 - 08:45; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:00 - 10:15; 10:15 - 10:30; 10:30 - 10:45; 11:45 - 12:00</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>DON HEBER CAFÉ</t>
+          <t>CAFE MIS TAITAS</t>
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C20" s="5" t="inlineStr">
         <is>
-          <t>5/5</t>
+          <t>1/1</t>
         </is>
       </c>
       <c r="D20" s="5" t="inlineStr">
         <is>
-          <t>ARMANDO VELÁSQUEZ; INMERSSO BOUTIQUE; BOX BRAND; REGIONAL S.A.S; INTERLINK2AMERICAS</t>
+          <t>INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="E20" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00</t>
+          <t>09:15 - 09:30</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="inlineStr">
         <is>
-          <t>SIETE LEONES CAFÉ</t>
+          <t>CAFÉ CAMPOHERMOSO</t>
         </is>
       </c>
       <c r="B21" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="5" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>2/2</t>
         </is>
       </c>
       <c r="D21" s="5" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS; BOX BRAND; INMERSSO BOUTIQUE</t>
+          <t>FLOR A FRUTO; NEIRA YORK COFFEE</t>
         </is>
       </c>
       <c r="E21" s="5" t="inlineStr">
         <is>
-          <t>09:30 - 09:45; 10:15 - 10:30; 10:30 - 10:45</t>
+          <t>08:30 - 08:45; 10:45 - 11:00</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ ERMITAÑO</t>
+          <t>CAFÉ MURAL</t>
         </is>
       </c>
       <c r="B22" s="5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C22" s="5" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>5/5</t>
         </is>
       </c>
       <c r="D22" s="5" t="inlineStr">
         <is>
-          <t>INMERSSO BOUTIQUE; FLOR A FRUTO; COLFRESH COFFEE</t>
+          <t>BOX BRAND; INTERLINK2AMERICAS; INMERSSO BOUTIQUE; COLFRESH COFFEE; NEIRA YORK COFFEE</t>
         </is>
       </c>
       <c r="E22" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15</t>
+          <t>08:45 - 09:00; 09:00 - 09:15; 09:30 - 09:45; 09:45 - 10:00; 11:00 - 11:15</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="inlineStr">
         <is>
-          <t>ROJO PASIÓN</t>
+          <t>FINCA LA FEDERICA</t>
         </is>
       </c>
       <c r="B23" s="5" t="n">
@@ -3206,119 +3277,119 @@
       </c>
       <c r="D23" s="5" t="inlineStr">
         <is>
-          <t>REGIONAL S.A.S; CAFÉ MOLINA; BOX BRAND; INMERSSO BOUTIQUE; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.; FLOR A FRUTO; NEIRA YORK COFFEE</t>
+          <t>REGIONAL S.A.S; CAFÉ MOLINA; INMERSSO BOUTIQUE; ARMANDO VELÁSQUEZ; COLFRESH COFFEE; INTERLINK2AMERICAS; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
         </is>
       </c>
       <c r="E23" s="5" t="inlineStr">
         <is>
-          <t>08:45 - 09:00; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:15 - 10:30; 10:45 - 11:00; 11:00 - 11:15</t>
+          <t>08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:30 - 10:45; 10:45 - 11:00</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="inlineStr">
         <is>
-          <t>RUNA COFFEE</t>
+          <t>D'CLEO COFFEE</t>
         </is>
       </c>
       <c r="B24" s="5" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C24" s="5" t="inlineStr">
         <is>
-          <t>8/8</t>
+          <t>3/3</t>
         </is>
       </c>
       <c r="D24" s="5" t="inlineStr">
         <is>
-          <t>BOX BRAND; COLFRESH COFFEE; CAFÉ MOLINA; INMERSSO BOUTIQUE; ARMANDO VELÁSQUEZ; FLOR A FRUTO; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.; NEIRA YORK COFFEE</t>
+          <t>BOX BRAND; INTERLINK2AMERICAS; PROCOLOMBIA</t>
         </is>
       </c>
       <c r="E24" s="5" t="inlineStr">
         <is>
-          <t>08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:15 - 10:30; 10:30 - 10:45; 10:45 - 11:00</t>
+          <t>08:30 - 08:45; 09:30 - 09:45; 12:00 - 12:15</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ OASIS DE SAMDA</t>
+          <t>CAFÉ ORIGEN DE LA MONTAÑA</t>
         </is>
       </c>
       <c r="B25" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C25" s="5" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>4/4</t>
         </is>
       </c>
       <c r="D25" s="5" t="inlineStr">
         <is>
-          <t>INMERSSO BOUTIQUE; FLOR A FRUTO; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
+          <t>BOX BRAND; INMERSSO BOUTIQUE; INTERLINK2AMERICAS; PROCOLOMBIA</t>
         </is>
       </c>
       <c r="E25" s="5" t="inlineStr">
         <is>
-          <t>10:30 - 10:45; 10:45 - 11:00; 11:00 - 11:15</t>
+          <t>11:15 - 11:30; 11:30 - 11:45; 11:45 - 12:00; 12:00 - 12:15</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ AGUA VIVA</t>
+          <t>SIETE LEONES CAFÉ</t>
         </is>
       </c>
       <c r="B26" s="5" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C26" s="5" t="inlineStr">
         <is>
-          <t>10/10</t>
+          <t>3/3</t>
         </is>
       </c>
       <c r="D26" s="5" t="inlineStr">
         <is>
-          <t>FLOR A FRUTO; CAFÉ MOLINA; REGIONAL S.A.S; ARMANDO VELÁSQUEZ; COLFRESH COFFEE; BOX BRAND; NEIRA YORK COFFEE; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.; INTERLINK2AMERICAS; INMERSSO BOUTIQUE</t>
+          <t>INTERLINK2AMERICAS; BOX BRAND; INMERSSO BOUTIQUE</t>
         </is>
       </c>
       <c r="E26" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:45 - 10:00; 10:00 - 10:15; 10:15 - 10:30; 11:00 - 11:15; 11:15 - 11:30; 11:45 - 12:00</t>
+          <t>09:15 - 09:30; 09:45 - 10:00; 10:00 - 10:15</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ MURAL</t>
+          <t>CAFE ARTE</t>
         </is>
       </c>
       <c r="B27" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C27" s="5" t="inlineStr">
         <is>
-          <t>5/5</t>
+          <t>2/2</t>
         </is>
       </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
-          <t>COLFRESH COFFEE; INMERSSO BOUTIQUE; INTERLINK2AMERICAS; BOX BRAND; NEIRA YORK COFFEE</t>
+          <t>PROCOLOMBIA; INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="E27" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 11:15 - 11:30</t>
+          <t>08:30 - 08:45; 09:30 - 09:45</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ VALLE DE LIRIO</t>
+          <t>CAFÉ AGUA VIVA</t>
         </is>
       </c>
       <c r="B28" s="5" t="n">
@@ -3331,112 +3402,137 @@
       </c>
       <c r="D28" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ MOLINA; ARMANDO VELÁSQUEZ; REGIONAL S.A.S; INMERSSO BOUTIQUE; BOX BRAND; COLFRESH COFFEE; FLOR A FRUTO; NEIRA YORK COFFEE; INTERLINK2AMERICAS; PROCOLOMBIA</t>
+          <t>INTERLINK2AMERICAS; COLFRESH COFFEE; CAFÉ MOLINA; REGIONAL S.A.S; FLOR A FRUTO; INMERSSO BOUTIQUE; ARMANDO VELÁSQUEZ; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.; BOX BRAND; NEIRA YORK COFFEE</t>
         </is>
       </c>
       <c r="E28" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:00 - 10:15; 11:00 - 11:15; 11:15 - 11:30; 12:00 - 12:15</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:45 - 10:00; 10:00 - 10:15; 10:15 - 10:30; 11:00 - 11:15; 11:15 - 11:30; 11:30 - 11:45</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ CAMPOHERMOSO</t>
+          <t>LADERAS DEL TAPIAS</t>
         </is>
       </c>
       <c r="B29" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C29" s="5" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>4/4</t>
         </is>
       </c>
       <c r="D29" s="5" t="inlineStr">
         <is>
-          <t>FLOR A FRUTO; NEIRA YORK COFFEE</t>
+          <t>ARMANDO VELÁSQUEZ; BOX BRAND; INMERSSO BOUTIQUE; INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="E29" s="5" t="inlineStr">
         <is>
-          <t>09:00 - 09:15; 10:30 - 10:45</t>
+          <t>08:30 - 08:45; 09:00 - 09:15; 09:30 - 09:45; 11:45 - 12:00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ MATILDE 1960</t>
+          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS</t>
         </is>
       </c>
       <c r="B30" s="5" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C30" s="5" t="inlineStr">
         <is>
-          <t>7/7</t>
+          <t>4/4</t>
         </is>
       </c>
       <c r="D30" s="5" t="inlineStr">
         <is>
-          <t>REGIONAL S.A.S; COLFRESH COFFEE; BOX BRAND; ARMANDO VELÁSQUEZ; INMERSSO BOUTIQUE; INTERLINK2AMERICAS; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
+          <t>INTERLINK2AMERICAS; REGIONAL S.A.S; BOX BRAND; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
         </is>
       </c>
       <c r="E30" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:30 - 10:45</t>
+          <t>08:45 - 09:00; 09:30 - 09:45; 09:45 - 10:00; 11:00 - 11:15</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="inlineStr">
         <is>
-          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS</t>
+          <t>DE SOL A SOL</t>
         </is>
       </c>
       <c r="B31" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" s="5" t="inlineStr">
         <is>
-          <t>4/4</t>
+          <t>5/5</t>
         </is>
       </c>
       <c r="D31" s="5" t="inlineStr">
         <is>
-          <t>REGIONAL S.A.S; BOX BRAND; INTERLINK2AMERICAS; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
+          <t>CAFÉ MOLINA; COLFRESH COFFEE; FLOR A FRUTO; ARMANDO VELÁSQUEZ; NEIRA YORK COFFEE</t>
         </is>
       </c>
       <c r="E31" s="5" t="inlineStr">
         <is>
-          <t>08:45 - 09:00; 09:30 - 09:45; 10:15 - 10:30; 10:45 - 11:00</t>
+          <t>08:30 - 08:45; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 11:30 - 11:45</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="inlineStr">
         <is>
-          <t>CAFE GRANEAO</t>
+          <t>ROJO PASIÓN</t>
         </is>
       </c>
       <c r="B32" s="5" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C32" s="5" t="inlineStr">
         <is>
-          <t>1/1</t>
+          <t>7/7</t>
         </is>
       </c>
       <c r="D32" s="5" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS</t>
+          <t>CAFÉ MOLINA; INMERSSO BOUTIQUE; REGIONAL S.A.S; BOX BRAND; ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.; FLOR A FRUTO; NEIRA YORK COFFEE</t>
         </is>
       </c>
       <c r="E32" s="5" t="inlineStr">
         <is>
-          <t>09:45 - 10:00</t>
+          <t>08:45 - 09:00; 09:00 - 09:15; 09:30 - 09:45; 09:45 - 10:00; 10:15 - 10:30; 10:30 - 10:45; 10:45 - 11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="inlineStr">
+        <is>
+          <t>CAFÉ LA AVANZANTE</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" s="5" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="D33" s="5" t="inlineStr">
+        <is>
+          <t>INMERSSO BOUTIQUE; NEIRA YORK COFFEE</t>
+        </is>
+      </c>
+      <c r="E33" s="5" t="inlineStr">
+        <is>
+          <t>08:30 - 08:45; 10:15 - 10:30</t>
         </is>
       </c>
     </row>
@@ -3490,80 +3586,80 @@
     <row r="2">
       <c r="A2" s="5" t="inlineStr">
         <is>
-          <t>FLOR A FRUTO</t>
+          <t>INTERLINK2AMERICAS</t>
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ AGUA VIVA; CAFÉ ARENILLO; SANTA CRUZ DE LAS AGUAS; CAFÉ ERMITAÑO; CAFÉ CAMPOHERMOSO; FINCA LA RIVERA; CAFE FINCA MI TERRON; CAFÉ VALLE DE LIRIO; DE SOL A SOL; RUNA COFFEE; DELUXE COFFEE; CAFÉ OASIS DE SAMDA; FINCA EL CASCABEL; ROJO PASIÓN</t>
+          <t>CAFÉ AGUA VIVA; CAFÉ ARENILLO; VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS; CAFÉ GRANADA; CAFÉ MURAL; DON HEBER CAFÉ; SIETE LEONES CAFÉ; LA PATRONA; CAFE MIS TAITAS; CAFÉ TRADICIÓN NEIRA; CAFE ARTE; D'CLEO COFFEE; CAFE FINCA MI TERRON; FINCA EL CASCABEL; SANTA CRUZ DE LAS AGUAS; CAFÉ VALLE DE LIRIO; CAFE GRANEAO; FINCA LA FEDERICA; DELUXE COFFEE; CAFÉ MATILDE 1960; CAFÉ ORIGEN DE LA MONTAÑA; FINCA LA RIVERA; LADERAS DEL TAPIAS</t>
         </is>
       </c>
       <c r="D2" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 10:00 - 10:15; 10:15 - 10:30; 10:45 - 11:00</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 10:00 - 10:15; 10:15 - 10:30; 10:30 - 10:45; 11:45 - 12:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
         <is>
-          <t>BOX BRAND</t>
+          <t>ARMANDO VELÁSQUEZ</t>
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>D'CLEO COFFEE; LADERAS DEL TAPIAS; RUNA COFFEE; CAFÉ MATILDE 1960; SANTA CRUZ DE LAS AGUAS; CAFE FINCA MI TERRON; DON HEBER CAFÉ; FINCA LA RIVERA; VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS; CAFÉ VALLE DE LIRIO; ROJO PASIÓN; FINCA EL CASCABEL; DELUXE COFFEE; CAFÉ MURAL; CAFÉ GRANADA; CAFÉ AGUA VIVA; CAFÉ TRADICIÓN NEIRA; SIETE LEONES CAFÉ; CAFE ARTE; CAFÉ ARENILLO; CAFÉ ORIGEN DE LA MONTAÑA</t>
+          <t>CINCO DAMAS; FINCA EL CASCABEL; LADERAS DEL TAPIAS; DON HEBER CAFÉ; CAFE FINCA MI TERRON; FINCA LA FEDERICA; DE SOL A SOL; DELUXE COFFEE; CAFÉ AGUA VIVA; CAFÉ MATILDE 1960; RUNA COFFEE; CAFÉ VALLE DE LIRIO</t>
         </is>
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:00 - 10:15; 10:15 - 10:30; 11:30 - 11:45</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:30 - 09:45; 10:15 - 10:30; 10:45 - 11:00</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ MOLINA</t>
+          <t>BOX BRAND</t>
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ VALLE DE LIRIO; DE SOL A SOL; FINCA LA RIVERA; CAFÉ AGUA VIVA; EL ORGASMO DE LOS SAINOS; DELUXE COFFEE; RUNA COFFEE; ROJO PASIÓN</t>
+          <t>D'CLEO COFFEE; CAFÉ MURAL; CAFÉ TRADICIÓN NEIRA; DELUXE COFFEE; LADERAS DEL TAPIAS; RUNA COFFEE; CAFE FINCA MI TERRON; CAFÉ VALLE DE LIRIO; FINCA EL CASCABEL; FINCA LA RIVERA; SIETE LEONES CAFÉ; ROJO PASIÓN; VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS; CAFÉ GRANADA; SANTA CRUZ DE LAS AGUAS; CAFÉ MATILDE 1960; CAFÉ ARENILLO; EL ORGASMO DE LOS SAINOS; CAFÉ AGUA VIVA; DON HEBER CAFÉ; CAFÉ ORIGEN DE LA MONTAÑA</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:00 - 10:15; 10:15 - 10:30; 11:15 - 11:30</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
+          <t>COLFRESH COFFEE</t>
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>ROJO PASIÓN; FINCA EL CASCABEL; CAFÉ MATILDE 1960; RUNA COFFEE; CAFÉ TRADICIÓN NEIRA; VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS; CAFÉ AGUA VIVA; CAFÉ OASIS DE SAMDA</t>
+          <t>CAFÉ ERMITAÑO; CAFÉ MATILDE 1960; CAFÉ VALLE DE LIRIO; CAFÉ AGUA VIVA; CAFÉ ARENILLO; DE SOL A SOL; EL ORGASMO DE LOS SAINOS; DELUXE COFFEE; LA PATRONA; CAFÉ MURAL; FINCA LA FEDERICA; FINCA LA RIVERA; RUNA COFFEE</t>
         </is>
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>10:15 - 10:30; 10:30 - 10:45; 10:45 - 11:00; 11:00 - 11:15</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:30 - 09:45; 09:45 - 10:00; 10:00 - 10:15</t>
         </is>
       </c>
     </row>
@@ -3578,12 +3674,12 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ MATILDE 1960; DELUXE COFFEE; VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS; ROJO PASIÓN; CAFÉ VALLE DE LIRIO; CAFÉ AGUA VIVA; EL ORGASMO DE LOS SAINOS; DON HEBER CAFÉ; FINCA LA RIVERA; CAFE ARTE</t>
+          <t>DELUXE COFFEE; DON HEBER CAFÉ; EL ORGASMO DE LOS SAINOS; CAFÉ MATILDE 1960; FINCA LA FEDERICA; CAFÉ VALLE DE LIRIO; CAFE FINCA MI TERRON; FINCA LA RIVERA; CAFÉ AGUA VIVA; VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS; ROJO PASIÓN</t>
         </is>
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:30 - 09:45; 09:45 - 10:00</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45</t>
         </is>
       </c>
     </row>
@@ -3598,32 +3694,32 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ ERMITAÑO; CAFÉ GRANADA; CINCO DAMAS; DON HEBER CAFÉ; CAFÉ LA AVANZANTE; CAFÉ TRADICIÓN NEIRA; DELUXE COFFEE; CAFÉ VALLE DE LIRIO; CAFÉ MURAL; RUNA COFFEE; CAFÉ MATILDE 1960; FINCA LA RIVERA; LADERAS DEL TAPIAS; ROJO PASIÓN; CAFÉ ARENILLO; SIETE LEONES CAFÉ; CAFÉ OASIS DE SAMDA; CAFÉ ORIGEN DE LA MONTAÑA; CAFÉ AGUA VIVA</t>
+          <t>CAFÉ GRANADA; CAFÉ LA AVANZANTE; RUNA COFFEE; CINCO DAMAS; FINCA LA RIVERA; ROJO PASIÓN; DELUXE COFFEE; FINCA LA FEDERICA; CAFÉ TRADICIÓN NEIRA; DON HEBER CAFÉ; LADERAS DEL TAPIAS; CAFÉ MURAL; CAFÉ ERMITAÑO; CAFÉ OASIS DE SAMDA; CAFÉ VALLE DE LIRIO; CAFÉ AGUA VIVA; CAFÉ ARENILLO; SIETE LEONES CAFÉ; CAFÉ MATILDE 1960; CAFÉ ORIGEN DE LA MONTAÑA</t>
         </is>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:30 - 10:45; 11:45 - 12:00</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:00 - 10:15; 11:30 - 11:45</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>COLFRESH COFFEE</t>
+          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>CAFÉ MURAL; EL ORGASMO DE LOS SAINOS; LA PATRONA; CAFÉ MATILDE 1960; DE SOL A SOL; CAFÉ ERMITAÑO; RUNA COFFEE; CAFÉ AGUA VIVA; CAFÉ VALLE DE LIRIO; CAFÉ ARENILLO; FINCA LA RIVERA; DELUXE COFFEE</t>
+          <t>ROJO PASIÓN; FINCA EL CASCABEL; CAFÉ OASIS DE SAMDA; RUNA COFFEE; FINCA LA FEDERICA; CAFÉ TRADICIÓN NEIRA; CAFÉ AGUA VIVA; VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS</t>
         </is>
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:45 - 10:00; 10:30 - 10:45</t>
+          <t>10:15 - 10:30; 10:30 - 10:45; 10:45 - 11:00; 11:00 - 11:15</t>
         </is>
       </c>
     </row>
@@ -3638,32 +3734,32 @@
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA; CAFE ARTE; CAFÉ LA AVANZANTE; D'CLEO COFFEE; EL ORGASMO DE LOS SAINOS; CAFÉ ORIGEN DE LA MONTAÑA; CAFÉ VALLE DE LIRIO</t>
+          <t>FINCA LA RIVERA; CAFE ARTE; CAFE FINCA MI TERRON; CAFÉ VALLE DE LIRIO; EL ORGASMO DE LOS SAINOS; CAFÉ ORIGEN DE LA MONTAÑA; D'CLEO COFFEE</t>
         </is>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 12:00 - 12:15</t>
+          <t>08:30 - 08:45; 10:00 - 10:15; 12:00 - 12:15</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="inlineStr">
         <is>
-          <t>INTERLINK2AMERICAS</t>
+          <t>CAFÉ MOLINA</t>
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>CAFE FINCA MI TERRON; CAFE MIS TAITAS; CAFÉ TRADICIÓN NEIRA; FINCA EL CASCABEL; LA PATRONA; D'CLEO COFFEE; CAFÉ GRANADA; SANTA CRUZ DE LAS AGUAS; LADERAS DEL TAPIAS; SIETE LEONES CAFÉ; CAFÉ MURAL; CAFE ARTE; CAFE GRANEAO; CAFÉ MATILDE 1960; DON HEBER CAFÉ; FINCA LA RIVERA; DELUXE COFFEE; CAFÉ ARENILLO; VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS; CAFÉ LA AVANZANTE; CAFÉ AGUA VIVA; CAFÉ ORIGEN DE LA MONTAÑA; CAFÉ VALLE DE LIRIO</t>
+          <t>CAFÉ VALLE DE LIRIO; DE SOL A SOL; DELUXE COFFEE; ROJO PASIÓN; FINCA LA FEDERICA; CAFÉ AGUA VIVA; EL ORGASMO DE LOS SAINOS; CAFE FINCA MI TERRON; RUNA COFFEE; FINCA LA RIVERA</t>
         </is>
       </c>
       <c r="D10" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:30 - 09:45; 09:45 - 10:00; 10:00 - 10:15; 10:15 - 10:30; 11:15 - 11:30</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:30 - 09:45; 09:45 - 10:00</t>
         </is>
       </c>
     </row>
@@ -3678,32 +3774,32 @@
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA; CAFÉ AGUA VIVA; CAFÉ CAMPOHERMOSO; CAFÉ LA AVANZANTE; CINCO DAMAS; RUNA COFFEE; ROJO PASIÓN; CAFÉ VALLE DE LIRIO; CAFÉ MURAL; DE SOL A SOL</t>
+          <t>CAFÉ LA AVANZANTE; RUNA COFFEE; CINCO DAMAS; FINCA LA RIVERA; ROJO PASIÓN; CAFÉ CAMPOHERMOSO; CAFÉ MURAL; CAFÉ VALLE DE LIRIO; DE SOL A SOL; CAFÉ AGUA VIVA</t>
         </is>
       </c>
       <c r="D11" s="5" t="inlineStr">
         <is>
-          <t>10:15 - 10:30; 10:30 - 10:45; 10:45 - 11:00; 11:00 - 11:15; 11:15 - 11:30</t>
+          <t>10:15 - 10:30; 10:30 - 10:45; 10:45 - 11:00; 11:00 - 11:15; 11:30 - 11:45</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="inlineStr">
         <is>
-          <t>ARMANDO VELÁSQUEZ</t>
+          <t>FLOR A FRUTO</t>
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="5" t="inlineStr">
         <is>
-          <t>CINCO DAMAS; DON HEBER CAFÉ; FINCA EL CASCABEL; CAFÉ VALLE DE LIRIO; DELUXE COFFEE; LADERAS DEL TAPIAS; DE SOL A SOL; CAFÉ MATILDE 1960; CAFÉ AGUA VIVA; RUNA COFFEE; CAFE FINCA MI TERRON</t>
+          <t>CAFÉ CAMPOHERMOSO; CAFÉ OASIS DE SAMDA; RUNA COFFEE; FINCA EL CASCABEL; CAFÉ ARENILLO; CAFÉ VALLE DE LIRIO; DE SOL A SOL; CAFÉ AGUA VIVA; CAFE FINCA MI TERRON; DELUXE COFFEE; FINCA LA RIVERA; CAFÉ ERMITAÑO; SANTA CRUZ DE LAS AGUAS; ROJO PASIÓN</t>
         </is>
       </c>
       <c r="D12" s="5" t="inlineStr">
         <is>
-          <t>08:30 - 08:45; 08:45 - 09:00; 09:00 - 09:15; 09:15 - 09:30; 09:45 - 10:00</t>
+          <t>08:30 - 08:45; 08:45 - 09:00; 09:15 - 09:30; 09:45 - 10:00; 10:15 - 10:30; 10:30 - 10:45</t>
         </is>
       </c>
     </row>
@@ -3729,15 +3825,15 @@
     <col width="16" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="41" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
     <col width="50" customWidth="1" min="5" max="5"/>
     <col width="50" customWidth="1" min="6" max="6"/>
     <col width="50" customWidth="1" min="7" max="7"/>
     <col width="50" customWidth="1" min="8" max="8"/>
-    <col width="48" customWidth="1" min="9" max="9"/>
-    <col width="50" customWidth="1" min="10" max="10"/>
-    <col width="38" customWidth="1" min="11" max="11"/>
-    <col width="48" customWidth="1" min="12" max="12"/>
+    <col width="50" customWidth="1" min="9" max="9"/>
+    <col width="48" customWidth="1" min="10" max="10"/>
+    <col width="33" customWidth="1" min="11" max="11"/>
+    <col width="50" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3748,57 +3844,57 @@
       </c>
       <c r="B1" s="4" t="inlineStr">
         <is>
+          <t>INTERLINK2AMERICAS</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>ARMANDO VELÁSQUEZ</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>BOX BRAND</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>COLFRESH COFFEE</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>REGIONAL S.A.S</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>INMERSSO BOUTIQUE</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>PROCOLOMBIA</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
+        <is>
+          <t>CAFÉ MOLINA</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>NEIRA YORK COFFEE</t>
+        </is>
+      </c>
+      <c r="L1" s="4" t="inlineStr">
+        <is>
           <t>FLOR A FRUTO</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>BOX BRAND</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>CAFÉ MOLINA</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
-        </is>
-      </c>
-      <c r="F1" s="4" t="inlineStr">
-        <is>
-          <t>REGIONAL S.A.S</t>
-        </is>
-      </c>
-      <c r="G1" s="4" t="inlineStr">
-        <is>
-          <t>INMERSSO BOUTIQUE</t>
-        </is>
-      </c>
-      <c r="H1" s="4" t="inlineStr">
-        <is>
-          <t>COLFRESH COFFEE</t>
-        </is>
-      </c>
-      <c r="I1" s="4" t="inlineStr">
-        <is>
-          <t>PROCOLOMBIA</t>
-        </is>
-      </c>
-      <c r="J1" s="4" t="inlineStr">
-        <is>
-          <t>INTERLINK2AMERICAS</t>
-        </is>
-      </c>
-      <c r="K1" s="4" t="inlineStr">
-        <is>
-          <t>NEIRA YORK COFFEE</t>
-        </is>
-      </c>
-      <c r="L1" s="4" t="inlineStr">
-        <is>
-          <t>ARMANDO VELÁSQUEZ</t>
         </is>
       </c>
     </row>
@@ -3815,44 +3911,44 @@
       </c>
       <c r="C2" s="9" t="inlineStr">
         <is>
+          <t>CINCO DAMAS, FINCA EL CASCABEL, LADERAS DEL TAPIAS</t>
+        </is>
+      </c>
+      <c r="D2" s="9" t="inlineStr">
+        <is>
           <t>D'CLEO COFFEE</t>
         </is>
       </c>
-      <c r="D2" s="9" t="inlineStr">
+      <c r="E2" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ ERMITAÑO, CAFÉ MATILDE 1960</t>
+        </is>
+      </c>
+      <c r="F2" s="9" t="inlineStr">
+        <is>
+          <t>DELUXE COFFEE, DON HEBER CAFÉ, EL ORGASMO DE LOS SAINOS</t>
+        </is>
+      </c>
+      <c r="G2" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ GRANADA, CAFÉ LA AVANZANTE</t>
+        </is>
+      </c>
+      <c r="H2" s="10" t="inlineStr"/>
+      <c r="I2" s="9" t="inlineStr">
+        <is>
+          <t>FINCA LA RIVERA, CAFE ARTE, CAFE FINCA MI TERRON</t>
+        </is>
+      </c>
+      <c r="J2" s="9" t="inlineStr">
         <is>
           <t>CAFÉ VALLE DE LIRIO, DE SOL A SOL</t>
-        </is>
-      </c>
-      <c r="E2" s="10" t="inlineStr"/>
-      <c r="F2" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ MATILDE 1960, DELUXE COFFEE</t>
-        </is>
-      </c>
-      <c r="G2" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ ERMITAÑO, CAFÉ GRANADA</t>
-        </is>
-      </c>
-      <c r="H2" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ MURAL, EL ORGASMO DE LOS SAINOS, LA PATRONA</t>
-        </is>
-      </c>
-      <c r="I2" s="9" t="inlineStr">
-        <is>
-          <t>FINCA LA RIVERA, CAFE ARTE, CAFÉ LA AVANZANTE</t>
-        </is>
-      </c>
-      <c r="J2" s="9" t="inlineStr">
-        <is>
-          <t>CAFE FINCA MI TERRON, CAFE MIS TAITAS, CAFÉ TRADICIÓN NEIRA</t>
         </is>
       </c>
       <c r="K2" s="10" t="inlineStr"/>
       <c r="L2" s="9" t="inlineStr">
         <is>
-          <t>CINCO DAMAS, DON HEBER CAFÉ, FINCA EL CASCABEL</t>
+          <t>CAFÉ CAMPOHERMOSO, CAFÉ OASIS DE SAMDA, RUNA COFFEE</t>
         </is>
       </c>
     </row>
@@ -3864,49 +3960,45 @@
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>SANTA CRUZ DE LAS AGUAS, CAFÉ ERMITAÑO</t>
+          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS, CAFÉ GRANADA</t>
         </is>
       </c>
       <c r="C3" s="9" t="inlineStr">
         <is>
-          <t>LADERAS DEL TAPIAS, RUNA COFFEE</t>
+          <t>DON HEBER CAFÉ, CAFE FINCA MI TERRON</t>
         </is>
       </c>
       <c r="D3" s="9" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA, CAFÉ AGUA VIVA</t>
-        </is>
-      </c>
-      <c r="E3" s="10" t="inlineStr"/>
+          <t>CAFÉ MURAL, CAFÉ TRADICIÓN NEIRA</t>
+        </is>
+      </c>
+      <c r="E3" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ VALLE DE LIRIO, CAFÉ AGUA VIVA</t>
+        </is>
+      </c>
       <c r="F3" s="9" t="inlineStr">
         <is>
-          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS, ROJO PASIÓN</t>
+          <t>CAFÉ MATILDE 1960, FINCA LA FEDERICA</t>
         </is>
       </c>
       <c r="G3" s="9" t="inlineStr">
         <is>
-          <t>CINCO DAMAS, DON HEBER CAFÉ</t>
-        </is>
-      </c>
-      <c r="H3" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ MATILDE 1960, DE SOL A SOL</t>
-        </is>
-      </c>
-      <c r="I3" s="9" t="inlineStr">
-        <is>
-          <t>D'CLEO COFFEE, EL ORGASMO DE LOS SAINOS</t>
-        </is>
-      </c>
+          <t>RUNA COFFEE, CINCO DAMAS</t>
+        </is>
+      </c>
+      <c r="H3" s="10" t="inlineStr"/>
+      <c r="I3" s="10" t="inlineStr"/>
       <c r="J3" s="9" t="inlineStr">
         <is>
-          <t>FINCA EL CASCABEL, LA PATRONA</t>
+          <t>DELUXE COFFEE, ROJO PASIÓN</t>
         </is>
       </c>
       <c r="K3" s="10" t="inlineStr"/>
       <c r="L3" s="9" t="inlineStr">
         <is>
-          <t>CAFÉ VALLE DE LIRIO, DELUXE COFFEE</t>
+          <t>FINCA EL CASCABEL, CAFÉ ARENILLO</t>
         </is>
       </c>
     </row>
@@ -3918,47 +4010,39 @@
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>CAFÉ CAMPOHERMOSO, FINCA LA RIVERA</t>
-        </is>
-      </c>
-      <c r="C4" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ MATILDE 1960, SANTA CRUZ DE LAS AGUAS</t>
-        </is>
-      </c>
+          <t>CAFÉ MURAL, DON HEBER CAFÉ</t>
+        </is>
+      </c>
+      <c r="C4" s="10" t="inlineStr"/>
       <c r="D4" s="9" t="inlineStr">
         <is>
-          <t>EL ORGASMO DE LOS SAINOS, DELUXE COFFEE</t>
-        </is>
-      </c>
-      <c r="E4" s="10" t="inlineStr"/>
+          <t>DELUXE COFFEE, LADERAS DEL TAPIAS</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ ARENILLO, DE SOL A SOL, EL ORGASMO DE LOS SAINOS</t>
+        </is>
+      </c>
       <c r="F4" s="9" t="inlineStr">
         <is>
-          <t>CAFÉ VALLE DE LIRIO, CAFÉ AGUA VIVA</t>
+          <t>CAFÉ VALLE DE LIRIO, CAFE FINCA MI TERRON</t>
         </is>
       </c>
       <c r="G4" s="9" t="inlineStr">
         <is>
-          <t>CAFÉ LA AVANZANTE, CAFÉ TRADICIÓN NEIRA</t>
-        </is>
-      </c>
-      <c r="H4" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ ERMITAÑO, RUNA COFFEE</t>
-        </is>
-      </c>
+          <t>FINCA LA RIVERA, ROJO PASIÓN</t>
+        </is>
+      </c>
+      <c r="H4" s="10" t="inlineStr"/>
       <c r="I4" s="10" t="inlineStr"/>
       <c r="J4" s="9" t="inlineStr">
         <is>
-          <t>D'CLEO COFFEE, CAFÉ GRANADA</t>
+          <t>FINCA LA FEDERICA, CAFÉ AGUA VIVA</t>
         </is>
       </c>
       <c r="K4" s="10" t="inlineStr"/>
-      <c r="L4" s="9" t="inlineStr">
-        <is>
-          <t>LADERAS DEL TAPIAS, DE SOL A SOL</t>
-        </is>
-      </c>
+      <c r="L4" s="10" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="8" t="inlineStr">
@@ -3966,35 +4050,35 @@
           <t>09:15 - 09:30</t>
         </is>
       </c>
-      <c r="B5" s="10" t="inlineStr"/>
-      <c r="C5" s="9" t="inlineStr">
-        <is>
-          <t>CAFE FINCA MI TERRON, DON HEBER CAFÉ, FINCA LA RIVERA</t>
-        </is>
-      </c>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>SIETE LEONES CAFÉ, LA PATRONA, CAFE MIS TAITAS</t>
+        </is>
+      </c>
+      <c r="C5" s="10" t="inlineStr"/>
       <c r="D5" s="9" t="inlineStr">
         <is>
-          <t>RUNA COFFEE, ROJO PASIÓN</t>
+          <t>RUNA COFFEE, CAFE FINCA MI TERRON</t>
         </is>
       </c>
       <c r="E5" s="10" t="inlineStr"/>
-      <c r="F5" s="10" t="inlineStr"/>
+      <c r="F5" s="9" t="inlineStr">
+        <is>
+          <t>FINCA LA RIVERA, CAFÉ AGUA VIVA</t>
+        </is>
+      </c>
       <c r="G5" s="9" t="inlineStr">
         <is>
-          <t>DELUXE COFFEE, CAFÉ VALLE DE LIRIO, CAFÉ MURAL</t>
+          <t>DELUXE COFFEE, FINCA LA FEDERICA, CAFÉ TRADICIÓN NEIRA</t>
         </is>
       </c>
       <c r="H5" s="10" t="inlineStr"/>
       <c r="I5" s="10" t="inlineStr"/>
-      <c r="J5" s="9" t="inlineStr">
-        <is>
-          <t>SANTA CRUZ DE LAS AGUAS, LADERAS DEL TAPIAS</t>
-        </is>
-      </c>
+      <c r="J5" s="10" t="inlineStr"/>
       <c r="K5" s="10" t="inlineStr"/>
       <c r="L5" s="9" t="inlineStr">
         <is>
-          <t>CAFÉ MATILDE 1960, CAFÉ AGUA VIVA</t>
+          <t>CAFÉ VALLE DE LIRIO, DE SOL A SOL</t>
         </is>
       </c>
     </row>
@@ -4004,29 +4088,41 @@
           <t>09:30 - 09:45</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr"/>
+      <c r="B6" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ TRADICIÓN NEIRA, CAFE ARTE, D'CLEO COFFEE</t>
+        </is>
+      </c>
       <c r="C6" s="9" t="inlineStr">
         <is>
-          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS, CAFÉ VALLE DE LIRIO, ROJO PASIÓN</t>
-        </is>
-      </c>
-      <c r="D6" s="10" t="inlineStr"/>
-      <c r="E6" s="10" t="inlineStr"/>
+          <t>FINCA LA FEDERICA, DE SOL A SOL</t>
+        </is>
+      </c>
+      <c r="D6" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ VALLE DE LIRIO, FINCA EL CASCABEL, FINCA LA RIVERA</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="inlineStr">
+        <is>
+          <t>DELUXE COFFEE, LA PATRONA</t>
+        </is>
+      </c>
       <c r="F6" s="9" t="inlineStr">
         <is>
-          <t>EL ORGASMO DE LOS SAINOS, DON HEBER CAFÉ</t>
+          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS, ROJO PASIÓN</t>
         </is>
       </c>
       <c r="G6" s="9" t="inlineStr">
         <is>
-          <t>RUNA COFFEE, CAFÉ MATILDE 1960, FINCA LA RIVERA</t>
+          <t>DON HEBER CAFÉ, LADERAS DEL TAPIAS, CAFÉ MURAL</t>
         </is>
       </c>
       <c r="H6" s="10" t="inlineStr"/>
       <c r="I6" s="10" t="inlineStr"/>
       <c r="J6" s="9" t="inlineStr">
         <is>
-          <t>SIETE LEONES CAFÉ, CAFÉ MURAL, CAFE ARTE</t>
+          <t>EL ORGASMO DE LOS SAINOS, CAFE FINCA MI TERRON</t>
         </is>
       </c>
       <c r="K6" s="10" t="inlineStr"/>
@@ -4039,38 +4135,34 @@
         </is>
       </c>
       <c r="B7" s="10" t="inlineStr"/>
-      <c r="C7" s="9" t="inlineStr">
-        <is>
-          <t>FINCA EL CASCABEL, DELUXE COFFEE, CAFÉ MURAL</t>
-        </is>
-      </c>
-      <c r="D7" s="10" t="inlineStr"/>
-      <c r="E7" s="10" t="inlineStr"/>
-      <c r="F7" s="9" t="inlineStr">
-        <is>
-          <t>FINCA LA RIVERA, CAFE ARTE</t>
-        </is>
-      </c>
+      <c r="C7" s="10" t="inlineStr"/>
+      <c r="D7" s="9" t="inlineStr">
+        <is>
+          <t>SIETE LEONES CAFÉ, ROJO PASIÓN, VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS</t>
+        </is>
+      </c>
+      <c r="E7" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ MURAL, FINCA LA FEDERICA</t>
+        </is>
+      </c>
+      <c r="F7" s="10" t="inlineStr"/>
       <c r="G7" s="9" t="inlineStr">
         <is>
-          <t>LADERAS DEL TAPIAS, ROJO PASIÓN</t>
-        </is>
-      </c>
-      <c r="H7" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ AGUA VIVA, CAFÉ VALLE DE LIRIO, CAFÉ ARENILLO</t>
-        </is>
-      </c>
+          <t>CAFÉ ERMITAÑO, CAFÉ OASIS DE SAMDA, CAFÉ VALLE DE LIRIO</t>
+        </is>
+      </c>
+      <c r="H7" s="10" t="inlineStr"/>
       <c r="I7" s="10" t="inlineStr"/>
       <c r="J7" s="9" t="inlineStr">
         <is>
-          <t>CAFE GRANEAO, CAFÉ MATILDE 1960, DON HEBER CAFÉ</t>
+          <t>RUNA COFFEE, FINCA LA RIVERA</t>
         </is>
       </c>
       <c r="K7" s="10" t="inlineStr"/>
       <c r="L7" s="9" t="inlineStr">
         <is>
-          <t>RUNA COFFEE, CAFE FINCA MI TERRON</t>
+          <t>CAFÉ AGUA VIVA, CAFE FINCA MI TERRON, DELUXE COFFEE</t>
         </is>
       </c>
     </row>
@@ -4082,25 +4174,33 @@
       </c>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>CAFE FINCA MI TERRON, CAFÉ VALLE DE LIRIO, DE SOL A SOL</t>
-        </is>
-      </c>
-      <c r="C8" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ GRANADA, CAFÉ AGUA VIVA, CAFÉ TRADICIÓN NEIRA</t>
-        </is>
-      </c>
-      <c r="D8" s="10" t="inlineStr"/>
-      <c r="E8" s="10" t="inlineStr"/>
+          <t>CAFE FINCA MI TERRON, FINCA EL CASCABEL</t>
+        </is>
+      </c>
+      <c r="C8" s="10" t="inlineStr"/>
+      <c r="D8" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ GRANADA, SANTA CRUZ DE LAS AGUAS, CAFÉ MATILDE 1960</t>
+        </is>
+      </c>
+      <c r="E8" s="9" t="inlineStr">
+        <is>
+          <t>FINCA LA RIVERA, RUNA COFFEE</t>
+        </is>
+      </c>
       <c r="F8" s="10" t="inlineStr"/>
-      <c r="G8" s="10" t="inlineStr"/>
+      <c r="G8" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ AGUA VIVA, CAFÉ ARENILLO, SIETE LEONES CAFÉ</t>
+        </is>
+      </c>
       <c r="H8" s="10" t="inlineStr"/>
-      <c r="I8" s="10" t="inlineStr"/>
-      <c r="J8" s="9" t="inlineStr">
-        <is>
-          <t>FINCA LA RIVERA, DELUXE COFFEE, CAFÉ ARENILLO</t>
-        </is>
-      </c>
+      <c r="I8" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ VALLE DE LIRIO, EL ORGASMO DE LOS SAINOS</t>
+        </is>
+      </c>
+      <c r="J8" s="10" t="inlineStr"/>
       <c r="K8" s="10" t="inlineStr"/>
       <c r="L8" s="10" t="inlineStr"/>
     </row>
@@ -4112,35 +4212,39 @@
       </c>
       <c r="B9" s="9" t="inlineStr">
         <is>
-          <t>RUNA COFFEE, DELUXE COFFEE</t>
+          <t>SANTA CRUZ DE LAS AGUAS, CAFÉ VALLE DE LIRIO, CAFE GRANEAO</t>
         </is>
       </c>
       <c r="C9" s="9" t="inlineStr">
         <is>
-          <t>SIETE LEONES CAFÉ, CAFE ARTE</t>
-        </is>
-      </c>
-      <c r="D9" s="10" t="inlineStr"/>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>ROJO PASIÓN, FINCA EL CASCABEL</t>
-        </is>
-      </c>
+          <t>DELUXE COFFEE, CAFÉ AGUA VIVA, CAFÉ MATILDE 1960</t>
+        </is>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ ARENILLO, EL ORGASMO DE LOS SAINOS</t>
+        </is>
+      </c>
+      <c r="E9" s="10" t="inlineStr"/>
       <c r="F9" s="10" t="inlineStr"/>
       <c r="G9" s="10" t="inlineStr"/>
-      <c r="H9" s="10" t="inlineStr"/>
+      <c r="H9" s="9" t="inlineStr">
+        <is>
+          <t>ROJO PASIÓN, FINCA EL CASCABEL</t>
+        </is>
+      </c>
       <c r="I9" s="10" t="inlineStr"/>
-      <c r="J9" s="9" t="inlineStr">
-        <is>
-          <t>VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS, CAFÉ LA AVANZANTE</t>
-        </is>
-      </c>
+      <c r="J9" s="10" t="inlineStr"/>
       <c r="K9" s="9" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA, CAFÉ AGUA VIVA</t>
-        </is>
-      </c>
-      <c r="L9" s="10" t="inlineStr"/>
+          <t>CAFÉ LA AVANZANTE, RUNA COFFEE</t>
+        </is>
+      </c>
+      <c r="L9" s="9" t="inlineStr">
+        <is>
+          <t>FINCA LA RIVERA, CAFÉ ERMITAÑO</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="inlineStr">
@@ -4148,33 +4252,33 @@
           <t>10:30 - 10:45</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr"/>
+      <c r="B10" s="9" t="inlineStr">
+        <is>
+          <t>FINCA LA FEDERICA, DELUXE COFFEE, CAFÉ MATILDE 1960</t>
+        </is>
+      </c>
       <c r="C10" s="10" t="inlineStr"/>
       <c r="D10" s="10" t="inlineStr"/>
-      <c r="E10" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ MATILDE 1960, RUNA COFFEE</t>
-        </is>
-      </c>
+      <c r="E10" s="10" t="inlineStr"/>
       <c r="F10" s="10" t="inlineStr"/>
-      <c r="G10" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ ARENILLO, SIETE LEONES CAFÉ, CAFÉ OASIS DE SAMDA</t>
-        </is>
-      </c>
+      <c r="G10" s="10" t="inlineStr"/>
       <c r="H10" s="9" t="inlineStr">
         <is>
-          <t>FINCA LA RIVERA, DELUXE COFFEE</t>
+          <t>CAFÉ OASIS DE SAMDA, RUNA COFFEE</t>
         </is>
       </c>
       <c r="I10" s="10" t="inlineStr"/>
       <c r="J10" s="10" t="inlineStr"/>
       <c r="K10" s="9" t="inlineStr">
         <is>
-          <t>CAFÉ CAMPOHERMOSO, CAFÉ LA AVANZANTE</t>
-        </is>
-      </c>
-      <c r="L10" s="10" t="inlineStr"/>
+          <t>CINCO DAMAS, FINCA LA RIVERA</t>
+        </is>
+      </c>
+      <c r="L10" s="9" t="inlineStr">
+        <is>
+          <t>SANTA CRUZ DE LAS AGUAS, ROJO PASIÓN</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="inlineStr">
@@ -4182,26 +4286,26 @@
           <t>10:45 - 11:00</t>
         </is>
       </c>
-      <c r="B11" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ OASIS DE SAMDA, FINCA EL CASCABEL, ROJO PASIÓN</t>
-        </is>
-      </c>
-      <c r="C11" s="10" t="inlineStr"/>
+      <c r="B11" s="10" t="inlineStr"/>
+      <c r="C11" s="9" t="inlineStr">
+        <is>
+          <t>RUNA COFFEE, CAFÉ VALLE DE LIRIO</t>
+        </is>
+      </c>
       <c r="D11" s="10" t="inlineStr"/>
-      <c r="E11" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ TRADICIÓN NEIRA, VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS</t>
-        </is>
-      </c>
+      <c r="E11" s="10" t="inlineStr"/>
       <c r="F11" s="10" t="inlineStr"/>
       <c r="G11" s="10" t="inlineStr"/>
-      <c r="H11" s="10" t="inlineStr"/>
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>FINCA LA FEDERICA, CAFÉ TRADICIÓN NEIRA</t>
+        </is>
+      </c>
       <c r="I11" s="10" t="inlineStr"/>
       <c r="J11" s="10" t="inlineStr"/>
       <c r="K11" s="9" t="inlineStr">
         <is>
-          <t>CINCO DAMAS, RUNA COFFEE</t>
+          <t>ROJO PASIÓN, CAFÉ CAMPOHERMOSO</t>
         </is>
       </c>
       <c r="L11" s="10" t="inlineStr"/>
@@ -4215,19 +4319,19 @@
       <c r="B12" s="10" t="inlineStr"/>
       <c r="C12" s="10" t="inlineStr"/>
       <c r="D12" s="10" t="inlineStr"/>
-      <c r="E12" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ AGUA VIVA, CAFÉ OASIS DE SAMDA</t>
-        </is>
-      </c>
+      <c r="E12" s="10" t="inlineStr"/>
       <c r="F12" s="10" t="inlineStr"/>
       <c r="G12" s="10" t="inlineStr"/>
-      <c r="H12" s="10" t="inlineStr"/>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ AGUA VIVA, VILLA CLARA IMPORTACIONES Y EXPORTACIONES SAS</t>
+        </is>
+      </c>
       <c r="I12" s="10" t="inlineStr"/>
       <c r="J12" s="10" t="inlineStr"/>
       <c r="K12" s="9" t="inlineStr">
         <is>
-          <t>ROJO PASIÓN, CAFÉ VALLE DE LIRIO</t>
+          <t>CAFÉ MURAL, CAFÉ VALLE DE LIRIO</t>
         </is>
       </c>
       <c r="L12" s="10" t="inlineStr"/>
@@ -4240,22 +4344,18 @@
       </c>
       <c r="B13" s="10" t="inlineStr"/>
       <c r="C13" s="10" t="inlineStr"/>
-      <c r="D13" s="10" t="inlineStr"/>
+      <c r="D13" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ AGUA VIVA, DON HEBER CAFÉ, CAFÉ ORIGEN DE LA MONTAÑA</t>
+        </is>
+      </c>
       <c r="E13" s="10" t="inlineStr"/>
       <c r="F13" s="10" t="inlineStr"/>
       <c r="G13" s="10" t="inlineStr"/>
       <c r="H13" s="10" t="inlineStr"/>
       <c r="I13" s="10" t="inlineStr"/>
-      <c r="J13" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ AGUA VIVA, CAFÉ ORIGEN DE LA MONTAÑA, CAFÉ VALLE DE LIRIO</t>
-        </is>
-      </c>
-      <c r="K13" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ MURAL, DE SOL A SOL</t>
-        </is>
-      </c>
+      <c r="J13" s="10" t="inlineStr"/>
+      <c r="K13" s="10" t="inlineStr"/>
       <c r="L13" s="10" t="inlineStr"/>
     </row>
     <row r="14">
@@ -4265,19 +4365,23 @@
         </is>
       </c>
       <c r="B14" s="10" t="inlineStr"/>
-      <c r="C14" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ ARENILLO, CAFÉ ORIGEN DE LA MONTAÑA</t>
-        </is>
-      </c>
+      <c r="C14" s="10" t="inlineStr"/>
       <c r="D14" s="10" t="inlineStr"/>
       <c r="E14" s="10" t="inlineStr"/>
       <c r="F14" s="10" t="inlineStr"/>
-      <c r="G14" s="10" t="inlineStr"/>
+      <c r="G14" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ MATILDE 1960, CAFÉ ORIGEN DE LA MONTAÑA</t>
+        </is>
+      </c>
       <c r="H14" s="10" t="inlineStr"/>
       <c r="I14" s="10" t="inlineStr"/>
       <c r="J14" s="10" t="inlineStr"/>
-      <c r="K14" s="10" t="inlineStr"/>
+      <c r="K14" s="9" t="inlineStr">
+        <is>
+          <t>DE SOL A SOL, CAFÉ AGUA VIVA</t>
+        </is>
+      </c>
       <c r="L14" s="10" t="inlineStr"/>
     </row>
     <row r="15">
@@ -4286,16 +4390,16 @@
           <t>11:45 - 12:00</t>
         </is>
       </c>
-      <c r="B15" s="10" t="inlineStr"/>
+      <c r="B15" s="9" t="inlineStr">
+        <is>
+          <t>CAFÉ ORIGEN DE LA MONTAÑA, FINCA LA RIVERA, LADERAS DEL TAPIAS</t>
+        </is>
+      </c>
       <c r="C15" s="10" t="inlineStr"/>
       <c r="D15" s="10" t="inlineStr"/>
       <c r="E15" s="10" t="inlineStr"/>
       <c r="F15" s="10" t="inlineStr"/>
-      <c r="G15" s="9" t="inlineStr">
-        <is>
-          <t>CAFÉ ORIGEN DE LA MONTAÑA, CAFÉ AGUA VIVA</t>
-        </is>
-      </c>
+      <c r="G15" s="10" t="inlineStr"/>
       <c r="H15" s="10" t="inlineStr"/>
       <c r="I15" s="10" t="inlineStr"/>
       <c r="J15" s="10" t="inlineStr"/>
@@ -4317,7 +4421,7 @@
       <c r="H16" s="10" t="inlineStr"/>
       <c r="I16" s="9" t="inlineStr">
         <is>
-          <t>CAFÉ ORIGEN DE LA MONTAÑA, CAFÉ VALLE DE LIRIO</t>
+          <t>CAFÉ ORIGEN DE LA MONTAÑA, D'CLEO COFFEE</t>
         </is>
       </c>
       <c r="J16" s="10" t="inlineStr"/>
@@ -4335,7 +4439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D139"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4345,7 +4449,7 @@
   <cols>
     <col width="47" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -5032,24 +5136,24 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="11" t="inlineStr">
+      <c r="A32" s="12" t="inlineStr">
         <is>
           <t>CAFÉ MATILDE 1960</t>
         </is>
       </c>
-      <c r="B32" s="11" t="inlineStr">
+      <c r="B32" s="12" t="inlineStr">
         <is>
           <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
         </is>
       </c>
-      <c r="C32" s="11" t="inlineStr">
-        <is>
-          <t>✓ Cumplida</t>
-        </is>
-      </c>
-      <c r="D32" s="11" t="inlineStr">
-        <is>
-          <t>SÍ</t>
+      <c r="C32" s="12" t="inlineStr">
+        <is>
+          <t>✗ No cumplida</t>
+        </is>
+      </c>
+      <c r="D32" s="12" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -7402,6 +7506,160 @@
         </is>
       </c>
       <c r="D139" s="11" t="inlineStr">
+        <is>
+          <t>SÍ</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="11" t="inlineStr">
+        <is>
+          <t>FINCA LA FEDERICA</t>
+        </is>
+      </c>
+      <c r="B140" s="11" t="inlineStr">
+        <is>
+          <t>INTERLINK2AMERICAS</t>
+        </is>
+      </c>
+      <c r="C140" s="11" t="inlineStr">
+        <is>
+          <t>✓ Cumplida</t>
+        </is>
+      </c>
+      <c r="D140" s="11" t="inlineStr">
+        <is>
+          <t>SÍ</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="11" t="inlineStr">
+        <is>
+          <t>FINCA LA FEDERICA</t>
+        </is>
+      </c>
+      <c r="B141" s="11" t="inlineStr">
+        <is>
+          <t>INMERSSO BOUTIQUE</t>
+        </is>
+      </c>
+      <c r="C141" s="11" t="inlineStr">
+        <is>
+          <t>✓ Cumplida</t>
+        </is>
+      </c>
+      <c r="D141" s="11" t="inlineStr">
+        <is>
+          <t>SÍ</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="11" t="inlineStr">
+        <is>
+          <t>FINCA LA FEDERICA</t>
+        </is>
+      </c>
+      <c r="B142" s="11" t="inlineStr">
+        <is>
+          <t>CAFÉ MOLINA</t>
+        </is>
+      </c>
+      <c r="C142" s="11" t="inlineStr">
+        <is>
+          <t>✓ Cumplida</t>
+        </is>
+      </c>
+      <c r="D142" s="11" t="inlineStr">
+        <is>
+          <t>SÍ</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="11" t="inlineStr">
+        <is>
+          <t>FINCA LA FEDERICA</t>
+        </is>
+      </c>
+      <c r="B143" s="11" t="inlineStr">
+        <is>
+          <t>COLFRESH COFFEE</t>
+        </is>
+      </c>
+      <c r="C143" s="11" t="inlineStr">
+        <is>
+          <t>✓ Cumplida</t>
+        </is>
+      </c>
+      <c r="D143" s="11" t="inlineStr">
+        <is>
+          <t>SÍ</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="11" t="inlineStr">
+        <is>
+          <t>FINCA LA FEDERICA</t>
+        </is>
+      </c>
+      <c r="B144" s="11" t="inlineStr">
+        <is>
+          <t>REGIONAL S.A.S</t>
+        </is>
+      </c>
+      <c r="C144" s="11" t="inlineStr">
+        <is>
+          <t>✓ Cumplida</t>
+        </is>
+      </c>
+      <c r="D144" s="11" t="inlineStr">
+        <is>
+          <t>SÍ</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="11" t="inlineStr">
+        <is>
+          <t>FINCA LA FEDERICA</t>
+        </is>
+      </c>
+      <c r="B145" s="11" t="inlineStr">
+        <is>
+          <t>ENCADENAMIENTOS PRODUCTIVOS -  CAFE AROMAS DEL EJE / CAFÉ GRANEAO.</t>
+        </is>
+      </c>
+      <c r="C145" s="11" t="inlineStr">
+        <is>
+          <t>✓ Cumplida</t>
+        </is>
+      </c>
+      <c r="D145" s="11" t="inlineStr">
+        <is>
+          <t>SÍ</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="11" t="inlineStr">
+        <is>
+          <t>FINCA LA FEDERICA</t>
+        </is>
+      </c>
+      <c r="B146" s="11" t="inlineStr">
+        <is>
+          <t>ARMANDO VELÁSQUEZ</t>
+        </is>
+      </c>
+      <c r="C146" s="11" t="inlineStr">
+        <is>
+          <t>✓ Cumplida</t>
+        </is>
+      </c>
+      <c r="D146" s="11" t="inlineStr">
         <is>
           <t>SÍ</t>
         </is>

</xml_diff>